<commit_message>
added GPS unit tests
</commit_message>
<xml_diff>
--- a/src/main/java/ApplicationLayer/AppComponents/ExcelToAppComponent/Eolian_auriga/components.xlsx
+++ b/src/main/java/ApplicationLayer/AppComponents/ExcelToAppComponent/Eolian_auriga/components.xlsx
@@ -1,30 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Github\Eolian-Telemetria-Auriga\Protocol\src\ExcelToAppComponent\Eolian_auriga\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dante\Desktop\Eolian\Eolian-Auriga-backend\src\main\java\ApplicationLayer\AppComponents\ExcelToAppComponent\Eolian_auriga\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C02D1117-43D3-4C4C-A836-455D004E9B93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D2C5EA2-FDD1-4DE3-BEAE-5259B9CF989A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1704" yWindow="-108" windowWidth="21444" windowHeight="13176" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="inversor_der" sheetId="2" r:id="rId1"/>
     <sheet name="inversor_izq" sheetId="3" r:id="rId2"/>
     <sheet name="bms" sheetId="4" r:id="rId3"/>
-    <sheet name="bms_temp" sheetId="5" r:id="rId4"/>
-    <sheet name="bms_volt" sheetId="6" r:id="rId5"/>
-    <sheet name="luces" sheetId="11" r:id="rId6"/>
-    <sheet name="marchas" sheetId="12" r:id="rId7"/>
-    <sheet name="mppt1" sheetId="7" r:id="rId8"/>
-    <sheet name="mppt2" sheetId="8" r:id="rId9"/>
-    <sheet name="mppt3" sheetId="9" r:id="rId10"/>
-    <sheet name="mppt4" sheetId="10" r:id="rId11"/>
-    <sheet name="acelerometro" sheetId="14" r:id="rId12"/>
+    <sheet name="gps" sheetId="15" r:id="rId4"/>
+    <sheet name="bms_temp" sheetId="5" r:id="rId5"/>
+    <sheet name="bms_volt" sheetId="6" r:id="rId6"/>
+    <sheet name="luces" sheetId="11" r:id="rId7"/>
+    <sheet name="marchas" sheetId="12" r:id="rId8"/>
+    <sheet name="mppt1" sheetId="7" r:id="rId9"/>
+    <sheet name="mppt2" sheetId="8" r:id="rId10"/>
+    <sheet name="mppt3" sheetId="9" r:id="rId11"/>
+    <sheet name="mppt4" sheetId="10" r:id="rId12"/>
+    <sheet name="acelerometro" sheetId="14" r:id="rId13"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="128">
   <si>
     <t>SOC</t>
   </si>
@@ -396,6 +397,30 @@
   </si>
   <si>
     <t>marcha</t>
+  </si>
+  <si>
+    <t>LATITUD</t>
+  </si>
+  <si>
+    <t>ANGULO_LATITUD</t>
+  </si>
+  <si>
+    <t>ORIENTACION_LATITUD</t>
+  </si>
+  <si>
+    <t>LONGITUD</t>
+  </si>
+  <si>
+    <t>ANGULO_LONGITUD</t>
+  </si>
+  <si>
+    <t>ORIENTACION_LONGITUD</t>
+  </si>
+  <si>
+    <t>00.0000</t>
+  </si>
+  <si>
+    <t>60.0000</t>
   </si>
 </sst>
 </file>
@@ -445,10 +470,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -735,9 +761,9 @@
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -753,7 +779,7 @@
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -769,7 +795,7 @@
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -785,7 +811,7 @@
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C8" s="1"/>
     </row>
   </sheetData>
@@ -795,6 +821,99 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50FA06F7-36F4-4A7C-BFEF-6657330EB921}">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>-0.1</v>
+      </c>
+      <c r="B2">
+        <v>-0.1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>-0.1</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0</v>
+      </c>
+      <c r="H2" s="2">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>129.9</v>
+      </c>
+      <c r="B3">
+        <v>49.9</v>
+      </c>
+      <c r="C3" s="2">
+        <v>129.9</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1</v>
+      </c>
+      <c r="H3" s="2">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B05DA13-A9BE-4CFA-8886-CBABF9CA7C76}">
   <dimension ref="A1:H3"/>
   <sheetViews>
@@ -802,9 +921,9 @@
       <selection sqref="A1:H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>105</v>
       </c>
@@ -830,7 +949,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>-0.1</v>
       </c>
@@ -856,7 +975,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>129.9</v>
       </c>
@@ -887,7 +1006,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C67BBD65-0C1C-49CF-A495-01A07240720A}">
   <dimension ref="A1:H3"/>
   <sheetViews>
@@ -895,9 +1014,9 @@
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>105</v>
       </c>
@@ -923,7 +1042,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>-0.1</v>
       </c>
@@ -949,7 +1068,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>129.9</v>
       </c>
@@ -980,7 +1099,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B6D6F58-ED9D-4990-A7A0-D169D3D50964}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -988,7 +1107,7 @@
       <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1002,9 +1121,9 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1020,7 +1139,7 @@
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1036,7 +1155,7 @@
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -1061,13 +1180,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72B547D1-632A-4F3B-9A3A-887796921B5F}">
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1114,7 +1233,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1161,7 +1280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>100</v>
       </c>
@@ -1214,6 +1333,84 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A1E0C48-4D9D-42FB-AD62-5ACFC1B922CE}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>-1</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B3">
+        <v>90</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="E3">
+        <v>180</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="A2 D2" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E39D22A6-69A3-4C78-81BF-9DE38D1DB719}">
   <dimension ref="A1:BH3"/>
   <sheetViews>
@@ -1221,9 +1418,9 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1405,7 +1602,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>-9.9</v>
       </c>
@@ -1587,7 +1784,7 @@
         <v>-9.9</v>
       </c>
     </row>
-    <row r="3" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>89.9</v>
       </c>
@@ -1775,7 +1972,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EF960A0-F629-434E-B8CE-7DE56A6AF799}">
   <dimension ref="A1:AD3"/>
   <sheetViews>
@@ -1783,9 +1980,9 @@
       <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>75</v>
       </c>
@@ -1877,7 +2074,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2.4990000000000001</v>
       </c>
@@ -1969,7 +2166,7 @@
         <v>2.4990000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>4.2990000000000004</v>
       </c>
@@ -2067,7 +2264,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E95E6DB-D9D5-48CC-A526-6D3DD8646156}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -2075,9 +2272,9 @@
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>113</v>
       </c>
@@ -2097,7 +2294,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2117,7 +2314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2142,7 +2339,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD999E06-E2C4-46D8-ABB0-7BAF398617DF}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -2150,14 +2347,14 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2167,7 +2364,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60ED005C-EE4F-4655-A412-314A8EE2E525}">
   <dimension ref="A1:H3"/>
   <sheetViews>
@@ -2175,9 +2372,9 @@
       <selection sqref="A1:H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>105</v>
       </c>
@@ -2203,7 +2400,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>-0.1</v>
       </c>
@@ -2229,100 +2426,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>129.9</v>
-      </c>
-      <c r="B3">
-        <v>49.9</v>
-      </c>
-      <c r="C3" s="2">
-        <v>129.9</v>
-      </c>
-      <c r="D3" s="2">
-        <v>1</v>
-      </c>
-      <c r="E3" s="2">
-        <v>1</v>
-      </c>
-      <c r="F3" s="2">
-        <v>1</v>
-      </c>
-      <c r="G3" s="2">
-        <v>1</v>
-      </c>
-      <c r="H3" s="2">
-        <v>100</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50FA06F7-36F4-4A7C-BFEF-6657330EB921}">
-  <dimension ref="A1:H3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E1" t="s">
-        <v>109</v>
-      </c>
-      <c r="F1" t="s">
-        <v>110</v>
-      </c>
-      <c r="G1" t="s">
-        <v>111</v>
-      </c>
-      <c r="H1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>-0.1</v>
-      </c>
-      <c r="B2">
-        <v>-0.1</v>
-      </c>
-      <c r="C2" s="2">
-        <v>-0.1</v>
-      </c>
-      <c r="D2" s="2">
-        <v>0</v>
-      </c>
-      <c r="E2" s="2">
-        <v>0</v>
-      </c>
-      <c r="F2" s="2">
-        <v>0</v>
-      </c>
-      <c r="G2" s="2">
-        <v>0</v>
-      </c>
-      <c r="H2" s="2">
-        <v>-10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>129.9</v>
       </c>

</xml_diff>

<commit_message>
v1 of CanbusChannelReader. Implemented for BMS AppComponent. Added missing data in xlsx
</commit_message>
<xml_diff>
--- a/src/main/java/ApplicationLayer/AppComponents/ExcelToAppComponent/Eolian_auriga/components.xlsx
+++ b/src/main/java/ApplicationLayer/AppComponents/ExcelToAppComponent/Eolian_auriga/components.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Github\Eolian-Auriga-backend\src\main\java\ApplicationLayer\AppComponents\ExcelToAppComponent\Eolian_auriga\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Github\Eolian\Eolian-Auriga-backend\src\main\java\ApplicationLayer\AppComponents\ExcelToAppComponent\Eolian_auriga\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AC90849-521E-4C59-90DC-F45E58BF4D27}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B359B71E-9DBE-463F-83AB-A4BD15E9C9BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="16080" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5670" yWindow="1935" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mppt1" sheetId="7" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="425">
   <si>
     <t>Luz_alta</t>
   </si>
@@ -1312,6 +1312,9 @@
   </si>
   <si>
     <t>z</t>
+  </si>
+  <si>
+    <t>Disharge_overcurrent</t>
   </si>
 </sst>
 </file>
@@ -1633,8 +1636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60ED005C-EE4F-4655-A412-314A8EE2E525}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1817,15 +1820,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72B547D1-632A-4F3B-9A3A-887796921B5F}">
-  <dimension ref="A1:NZ4"/>
+  <dimension ref="A1:OA5"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="OA5" sqref="OA5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:390" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:391" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -1884,1120 +1887,1123 @@
         <v>25</v>
       </c>
       <c r="T1" t="s">
+        <v>424</v>
+      </c>
+      <c r="U1" t="s">
         <v>26</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>27</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>28</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>29</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>30</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>31</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>32</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>33</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>34</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>35</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>36</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>37</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>38</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>39</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>40</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>41</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>42</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>43</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>44</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>45</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>46</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>47</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>48</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>49</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>50</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>51</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>52</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>53</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>54</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>55</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AY1" t="s">
         <v>56</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AZ1" t="s">
         <v>57</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BA1" t="s">
         <v>58</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BB1" t="s">
         <v>59</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BC1" t="s">
         <v>60</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BD1" t="s">
         <v>98</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BE1" t="s">
         <v>99</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BF1" t="s">
         <v>100</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BG1" t="s">
         <v>101</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BH1" t="s">
         <v>102</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BI1" t="s">
         <v>103</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BJ1" t="s">
         <v>104</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BK1" t="s">
         <v>105</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BL1" t="s">
         <v>106</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BM1" t="s">
         <v>107</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BN1" t="s">
         <v>108</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="BO1" t="s">
         <v>109</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="BP1" t="s">
         <v>110</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="BQ1" t="s">
         <v>111</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="BR1" t="s">
         <v>112</v>
       </c>
-      <c r="BR1" t="s">
+      <c r="BS1" t="s">
         <v>113</v>
       </c>
-      <c r="BS1" t="s">
+      <c r="BT1" t="s">
         <v>114</v>
       </c>
-      <c r="BT1" t="s">
+      <c r="BU1" t="s">
         <v>115</v>
       </c>
-      <c r="BU1" t="s">
+      <c r="BV1" t="s">
         <v>116</v>
       </c>
-      <c r="BV1" t="s">
+      <c r="BW1" t="s">
         <v>117</v>
       </c>
-      <c r="BW1" t="s">
+      <c r="BX1" t="s">
         <v>118</v>
       </c>
-      <c r="BX1" t="s">
+      <c r="BY1" t="s">
         <v>119</v>
       </c>
-      <c r="BY1" t="s">
+      <c r="BZ1" t="s">
         <v>120</v>
       </c>
-      <c r="BZ1" t="s">
+      <c r="CA1" t="s">
         <v>121</v>
       </c>
-      <c r="CA1" t="s">
+      <c r="CB1" t="s">
         <v>122</v>
       </c>
-      <c r="CB1" t="s">
+      <c r="CC1" t="s">
         <v>123</v>
       </c>
-      <c r="CC1" t="s">
+      <c r="CD1" t="s">
         <v>124</v>
       </c>
-      <c r="CD1" t="s">
+      <c r="CE1" t="s">
         <v>125</v>
       </c>
-      <c r="CE1" t="s">
+      <c r="CF1" t="s">
         <v>126</v>
       </c>
-      <c r="CF1" t="s">
+      <c r="CG1" t="s">
         <v>127</v>
       </c>
-      <c r="CG1" t="s">
+      <c r="CH1" t="s">
         <v>128</v>
       </c>
-      <c r="CH1" t="s">
+      <c r="CI1" t="s">
         <v>129</v>
       </c>
-      <c r="CI1" t="s">
+      <c r="CJ1" t="s">
         <v>130</v>
       </c>
-      <c r="CJ1" t="s">
+      <c r="CK1" t="s">
         <v>131</v>
       </c>
-      <c r="CK1" t="s">
+      <c r="CL1" t="s">
         <v>132</v>
       </c>
-      <c r="CL1" t="s">
+      <c r="CM1" t="s">
         <v>133</v>
       </c>
-      <c r="CM1" t="s">
+      <c r="CN1" t="s">
         <v>134</v>
       </c>
-      <c r="CN1" t="s">
+      <c r="CO1" t="s">
         <v>135</v>
       </c>
-      <c r="CO1" t="s">
+      <c r="CP1" t="s">
         <v>136</v>
       </c>
-      <c r="CP1" t="s">
+      <c r="CQ1" t="s">
         <v>137</v>
       </c>
-      <c r="CQ1" t="s">
+      <c r="CR1" t="s">
         <v>138</v>
       </c>
-      <c r="CR1" t="s">
+      <c r="CS1" t="s">
         <v>139</v>
       </c>
-      <c r="CS1" t="s">
+      <c r="CT1" t="s">
         <v>140</v>
       </c>
-      <c r="CT1" t="s">
+      <c r="CU1" t="s">
         <v>141</v>
       </c>
-      <c r="CU1" t="s">
+      <c r="CV1" t="s">
         <v>142</v>
       </c>
-      <c r="CV1" t="s">
+      <c r="CW1" t="s">
         <v>143</v>
       </c>
-      <c r="CW1" t="s">
+      <c r="CX1" t="s">
         <v>144</v>
       </c>
-      <c r="CX1" t="s">
+      <c r="CY1" t="s">
         <v>145</v>
       </c>
-      <c r="CY1" t="s">
+      <c r="CZ1" t="s">
         <v>146</v>
       </c>
-      <c r="CZ1" t="s">
+      <c r="DA1" t="s">
         <v>147</v>
       </c>
-      <c r="DA1" t="s">
+      <c r="DB1" t="s">
         <v>148</v>
       </c>
-      <c r="DB1" t="s">
+      <c r="DC1" t="s">
         <v>149</v>
       </c>
-      <c r="DC1" t="s">
+      <c r="DD1" t="s">
         <v>150</v>
       </c>
-      <c r="DD1" t="s">
+      <c r="DE1" t="s">
         <v>151</v>
       </c>
-      <c r="DE1" t="s">
+      <c r="DF1" t="s">
         <v>152</v>
       </c>
-      <c r="DF1" t="s">
+      <c r="DG1" t="s">
         <v>153</v>
       </c>
-      <c r="DG1" t="s">
+      <c r="DH1" t="s">
         <v>154</v>
       </c>
-      <c r="DH1" t="s">
+      <c r="DI1" t="s">
         <v>155</v>
       </c>
-      <c r="DI1" t="s">
+      <c r="DJ1" t="s">
         <v>156</v>
       </c>
-      <c r="DJ1" t="s">
+      <c r="DK1" t="s">
         <v>157</v>
       </c>
-      <c r="DK1" t="s">
+      <c r="DL1" t="s">
         <v>158</v>
       </c>
-      <c r="DL1" t="s">
+      <c r="DM1" t="s">
         <v>159</v>
       </c>
-      <c r="DM1" t="s">
+      <c r="DN1" t="s">
         <v>160</v>
       </c>
-      <c r="DN1" t="s">
+      <c r="DO1" t="s">
         <v>161</v>
       </c>
-      <c r="DO1" t="s">
+      <c r="DP1" t="s">
         <v>162</v>
       </c>
-      <c r="DP1" t="s">
+      <c r="DQ1" t="s">
         <v>163</v>
       </c>
-      <c r="DQ1" t="s">
+      <c r="DR1" t="s">
         <v>164</v>
       </c>
-      <c r="DR1" t="s">
+      <c r="DS1" t="s">
         <v>165</v>
       </c>
-      <c r="DS1" t="s">
+      <c r="DT1" t="s">
         <v>166</v>
       </c>
-      <c r="DT1" t="s">
+      <c r="DU1" t="s">
         <v>167</v>
       </c>
-      <c r="DU1" t="s">
+      <c r="DV1" t="s">
         <v>168</v>
       </c>
-      <c r="DV1" t="s">
+      <c r="DW1" t="s">
         <v>169</v>
       </c>
-      <c r="DW1" t="s">
+      <c r="DX1" t="s">
         <v>170</v>
       </c>
-      <c r="DX1" t="s">
+      <c r="DY1" t="s">
         <v>171</v>
       </c>
-      <c r="DY1" t="s">
+      <c r="DZ1" t="s">
         <v>172</v>
       </c>
-      <c r="DZ1" t="s">
+      <c r="EA1" t="s">
         <v>173</v>
       </c>
-      <c r="EA1" t="s">
+      <c r="EB1" t="s">
         <v>174</v>
       </c>
-      <c r="EB1" t="s">
+      <c r="EC1" t="s">
         <v>175</v>
       </c>
-      <c r="EC1" t="s">
+      <c r="ED1" t="s">
         <v>176</v>
       </c>
-      <c r="ED1" t="s">
+      <c r="EE1" t="s">
         <v>177</v>
       </c>
-      <c r="EE1" t="s">
+      <c r="EF1" t="s">
         <v>178</v>
       </c>
-      <c r="EF1" t="s">
+      <c r="EG1" t="s">
         <v>179</v>
       </c>
-      <c r="EG1" t="s">
+      <c r="EH1" t="s">
         <v>180</v>
       </c>
-      <c r="EH1" t="s">
+      <c r="EI1" t="s">
         <v>181</v>
       </c>
-      <c r="EI1" t="s">
+      <c r="EJ1" t="s">
         <v>182</v>
       </c>
-      <c r="EJ1" t="s">
+      <c r="EK1" t="s">
         <v>183</v>
       </c>
-      <c r="EK1" t="s">
+      <c r="EL1" t="s">
         <v>184</v>
       </c>
-      <c r="EL1" t="s">
+      <c r="EM1" t="s">
         <v>185</v>
       </c>
-      <c r="EM1" t="s">
+      <c r="EN1" t="s">
         <v>186</v>
       </c>
-      <c r="EN1" t="s">
+      <c r="EO1" t="s">
         <v>187</v>
       </c>
-      <c r="EO1" t="s">
+      <c r="EP1" t="s">
         <v>188</v>
       </c>
-      <c r="EP1" t="s">
+      <c r="EQ1" t="s">
         <v>189</v>
       </c>
-      <c r="EQ1" t="s">
+      <c r="ER1" t="s">
         <v>190</v>
       </c>
-      <c r="ER1" t="s">
+      <c r="ES1" t="s">
         <v>191</v>
       </c>
-      <c r="ES1" t="s">
+      <c r="ET1" t="s">
         <v>192</v>
       </c>
-      <c r="ET1" t="s">
+      <c r="EU1" t="s">
         <v>193</v>
       </c>
-      <c r="EU1" t="s">
+      <c r="EV1" t="s">
         <v>194</v>
       </c>
-      <c r="EV1" t="s">
+      <c r="EW1" t="s">
         <v>195</v>
       </c>
-      <c r="EW1" t="s">
+      <c r="EX1" t="s">
         <v>196</v>
       </c>
-      <c r="EX1" t="s">
+      <c r="EY1" t="s">
         <v>197</v>
       </c>
-      <c r="EY1" t="s">
+      <c r="EZ1" t="s">
         <v>198</v>
       </c>
-      <c r="EZ1" t="s">
+      <c r="FA1" t="s">
         <v>199</v>
       </c>
-      <c r="FA1" t="s">
+      <c r="FB1" t="s">
         <v>200</v>
       </c>
-      <c r="FB1" t="s">
+      <c r="FC1" t="s">
         <v>201</v>
       </c>
-      <c r="FC1" t="s">
+      <c r="FD1" t="s">
         <v>202</v>
       </c>
-      <c r="FD1" t="s">
+      <c r="FE1" t="s">
         <v>203</v>
       </c>
-      <c r="FE1" t="s">
+      <c r="FF1" t="s">
         <v>204</v>
       </c>
-      <c r="FF1" t="s">
+      <c r="FG1" t="s">
         <v>205</v>
       </c>
-      <c r="FG1" t="s">
+      <c r="FH1" t="s">
         <v>206</v>
       </c>
-      <c r="FH1" t="s">
+      <c r="FI1" t="s">
         <v>207</v>
       </c>
-      <c r="FI1" t="s">
+      <c r="FJ1" t="s">
         <v>208</v>
       </c>
-      <c r="FJ1" t="s">
+      <c r="FK1" t="s">
         <v>209</v>
       </c>
-      <c r="FK1" t="s">
+      <c r="FL1" t="s">
         <v>210</v>
       </c>
-      <c r="FL1" t="s">
+      <c r="FM1" t="s">
         <v>211</v>
       </c>
-      <c r="FM1" t="s">
+      <c r="FN1" t="s">
         <v>212</v>
       </c>
-      <c r="FN1" t="s">
+      <c r="FO1" t="s">
         <v>213</v>
       </c>
-      <c r="FO1" t="s">
+      <c r="FP1" t="s">
         <v>214</v>
       </c>
-      <c r="FP1" t="s">
+      <c r="FQ1" t="s">
         <v>215</v>
       </c>
-      <c r="FQ1" t="s">
+      <c r="FR1" t="s">
         <v>216</v>
       </c>
-      <c r="FR1" t="s">
+      <c r="FS1" t="s">
         <v>217</v>
       </c>
-      <c r="FS1" t="s">
+      <c r="FT1" t="s">
         <v>218</v>
       </c>
-      <c r="FT1" t="s">
+      <c r="FU1" t="s">
         <v>219</v>
       </c>
-      <c r="FU1" t="s">
+      <c r="FV1" t="s">
         <v>220</v>
       </c>
-      <c r="FV1" t="s">
+      <c r="FW1" t="s">
         <v>221</v>
       </c>
-      <c r="FW1" t="s">
+      <c r="FX1" t="s">
         <v>222</v>
       </c>
-      <c r="FX1" t="s">
+      <c r="FY1" t="s">
         <v>223</v>
       </c>
-      <c r="FY1" t="s">
+      <c r="FZ1" t="s">
         <v>224</v>
       </c>
-      <c r="FZ1" t="s">
+      <c r="GA1" t="s">
         <v>225</v>
       </c>
-      <c r="GA1" t="s">
+      <c r="GB1" t="s">
         <v>226</v>
       </c>
-      <c r="GB1" t="s">
+      <c r="GC1" t="s">
         <v>227</v>
       </c>
-      <c r="GC1" t="s">
+      <c r="GD1" t="s">
         <v>228</v>
       </c>
-      <c r="GD1" t="s">
+      <c r="GE1" t="s">
         <v>229</v>
       </c>
-      <c r="GE1" t="s">
+      <c r="GF1" t="s">
         <v>230</v>
       </c>
-      <c r="GF1" t="s">
+      <c r="GG1" t="s">
         <v>231</v>
       </c>
-      <c r="GG1" t="s">
+      <c r="GH1" t="s">
         <v>232</v>
       </c>
-      <c r="GH1" t="s">
+      <c r="GI1" t="s">
         <v>233</v>
       </c>
-      <c r="GI1" t="s">
+      <c r="GJ1" t="s">
         <v>234</v>
       </c>
-      <c r="GJ1" t="s">
+      <c r="GK1" t="s">
         <v>235</v>
       </c>
-      <c r="GK1" t="s">
+      <c r="GL1" t="s">
         <v>236</v>
       </c>
-      <c r="GL1" t="s">
+      <c r="GM1" t="s">
         <v>237</v>
       </c>
-      <c r="GM1" t="s">
+      <c r="GN1" t="s">
         <v>238</v>
       </c>
-      <c r="GN1" t="s">
+      <c r="GO1" t="s">
         <v>239</v>
       </c>
-      <c r="GO1" t="s">
+      <c r="GP1" t="s">
         <v>240</v>
       </c>
-      <c r="GP1" t="s">
+      <c r="GQ1" t="s">
         <v>241</v>
       </c>
-      <c r="GQ1" t="s">
+      <c r="GR1" t="s">
         <v>242</v>
       </c>
-      <c r="GR1" t="s">
+      <c r="GS1" t="s">
         <v>243</v>
       </c>
-      <c r="GS1" t="s">
+      <c r="GT1" t="s">
         <v>244</v>
       </c>
-      <c r="GT1" t="s">
+      <c r="GU1" t="s">
         <v>245</v>
       </c>
-      <c r="GU1" t="s">
+      <c r="GV1" t="s">
         <v>246</v>
       </c>
-      <c r="GV1" t="s">
+      <c r="GW1" t="s">
         <v>247</v>
       </c>
-      <c r="GW1" t="s">
+      <c r="GX1" t="s">
         <v>248</v>
       </c>
-      <c r="GX1" t="s">
+      <c r="GY1" t="s">
         <v>249</v>
       </c>
-      <c r="GY1" t="s">
+      <c r="GZ1" t="s">
         <v>250</v>
       </c>
-      <c r="GZ1" t="s">
+      <c r="HA1" t="s">
         <v>251</v>
       </c>
-      <c r="HA1" t="s">
+      <c r="HB1" t="s">
         <v>252</v>
       </c>
-      <c r="HB1" t="s">
+      <c r="HC1" t="s">
         <v>253</v>
       </c>
-      <c r="HC1" t="s">
+      <c r="HD1" t="s">
         <v>254</v>
       </c>
-      <c r="HD1" t="s">
+      <c r="HE1" t="s">
         <v>255</v>
       </c>
-      <c r="HE1" t="s">
+      <c r="HF1" t="s">
         <v>256</v>
       </c>
-      <c r="HF1" t="s">
+      <c r="HG1" t="s">
         <v>257</v>
       </c>
-      <c r="HG1" t="s">
+      <c r="HH1" t="s">
         <v>258</v>
       </c>
-      <c r="HH1" t="s">
+      <c r="HI1" t="s">
         <v>259</v>
       </c>
-      <c r="HI1" t="s">
+      <c r="HJ1" t="s">
         <v>260</v>
       </c>
-      <c r="HJ1" t="s">
+      <c r="HK1" t="s">
         <v>261</v>
       </c>
-      <c r="HK1" t="s">
+      <c r="HL1" t="s">
         <v>262</v>
       </c>
-      <c r="HL1" t="s">
+      <c r="HM1" t="s">
         <v>263</v>
       </c>
-      <c r="HM1" t="s">
+      <c r="HN1" t="s">
         <v>264</v>
       </c>
-      <c r="HN1" t="s">
+      <c r="HO1" t="s">
         <v>265</v>
       </c>
-      <c r="HO1" t="s">
+      <c r="HP1" t="s">
         <v>266</v>
       </c>
-      <c r="HP1" t="s">
+      <c r="HQ1" t="s">
         <v>267</v>
       </c>
-      <c r="HQ1" t="s">
+      <c r="HR1" t="s">
         <v>268</v>
       </c>
-      <c r="HR1" t="s">
+      <c r="HS1" t="s">
         <v>269</v>
       </c>
-      <c r="HS1" t="s">
+      <c r="HT1" t="s">
         <v>270</v>
       </c>
-      <c r="HT1" t="s">
+      <c r="HU1" t="s">
         <v>271</v>
       </c>
-      <c r="HU1" t="s">
+      <c r="HV1" t="s">
         <v>272</v>
       </c>
-      <c r="HV1" t="s">
+      <c r="HW1" t="s">
         <v>273</v>
       </c>
-      <c r="HW1" t="s">
+      <c r="HX1" t="s">
         <v>274</v>
       </c>
-      <c r="HX1" t="s">
+      <c r="HY1" t="s">
         <v>275</v>
       </c>
-      <c r="HY1" t="s">
+      <c r="HZ1" t="s">
         <v>276</v>
       </c>
-      <c r="HZ1" t="s">
+      <c r="IA1" t="s">
         <v>277</v>
       </c>
-      <c r="IA1" t="s">
+      <c r="IB1" t="s">
         <v>278</v>
       </c>
-      <c r="IB1" t="s">
+      <c r="IC1" t="s">
         <v>279</v>
       </c>
-      <c r="IC1" t="s">
+      <c r="ID1" t="s">
         <v>280</v>
       </c>
-      <c r="ID1" t="s">
+      <c r="IE1" t="s">
         <v>281</v>
       </c>
-      <c r="IE1" t="s">
+      <c r="IF1" t="s">
         <v>282</v>
       </c>
-      <c r="IF1" t="s">
+      <c r="IG1" t="s">
         <v>283</v>
       </c>
-      <c r="IG1" t="s">
+      <c r="IH1" t="s">
         <v>284</v>
       </c>
-      <c r="IH1" t="s">
+      <c r="II1" t="s">
         <v>285</v>
       </c>
-      <c r="II1" t="s">
+      <c r="IJ1" t="s">
         <v>286</v>
       </c>
-      <c r="IJ1" t="s">
+      <c r="IK1" t="s">
         <v>287</v>
       </c>
-      <c r="IK1" t="s">
+      <c r="IL1" t="s">
         <v>288</v>
       </c>
-      <c r="IL1" t="s">
+      <c r="IM1" t="s">
         <v>289</v>
       </c>
-      <c r="IM1" t="s">
+      <c r="IN1" t="s">
         <v>290</v>
       </c>
-      <c r="IN1" t="s">
+      <c r="IO1" t="s">
         <v>291</v>
       </c>
-      <c r="IO1" t="s">
+      <c r="IP1" t="s">
         <v>292</v>
       </c>
-      <c r="IP1" t="s">
+      <c r="IQ1" t="s">
         <v>293</v>
       </c>
-      <c r="IQ1" t="s">
+      <c r="IR1" t="s">
         <v>294</v>
       </c>
-      <c r="IR1" t="s">
+      <c r="IS1" t="s">
         <v>295</v>
       </c>
-      <c r="IS1" t="s">
+      <c r="IT1" t="s">
         <v>296</v>
       </c>
-      <c r="IT1" t="s">
+      <c r="IU1" t="s">
         <v>297</v>
       </c>
-      <c r="IU1" t="s">
+      <c r="IV1" t="s">
         <v>298</v>
       </c>
-      <c r="IV1" t="s">
+      <c r="IW1" t="s">
         <v>299</v>
       </c>
-      <c r="IW1" t="s">
+      <c r="IX1" t="s">
         <v>300</v>
       </c>
-      <c r="IX1" t="s">
+      <c r="IY1" t="s">
         <v>301</v>
       </c>
-      <c r="IY1" t="s">
+      <c r="IZ1" t="s">
         <v>302</v>
       </c>
-      <c r="IZ1" t="s">
+      <c r="JA1" t="s">
         <v>303</v>
       </c>
-      <c r="JA1" t="s">
+      <c r="JB1" t="s">
         <v>304</v>
       </c>
-      <c r="JB1" t="s">
+      <c r="JC1" t="s">
         <v>305</v>
       </c>
-      <c r="JC1" t="s">
+      <c r="JD1" t="s">
         <v>306</v>
       </c>
-      <c r="JD1" t="s">
+      <c r="JE1" t="s">
         <v>307</v>
       </c>
-      <c r="JE1" t="s">
+      <c r="JF1" t="s">
         <v>308</v>
       </c>
-      <c r="JF1" t="s">
+      <c r="JG1" t="s">
         <v>309</v>
       </c>
-      <c r="JG1" t="s">
+      <c r="JH1" t="s">
         <v>310</v>
       </c>
-      <c r="JH1" t="s">
+      <c r="JI1" t="s">
         <v>311</v>
       </c>
-      <c r="JI1" t="s">
+      <c r="JJ1" t="s">
         <v>312</v>
       </c>
-      <c r="JJ1" t="s">
+      <c r="JK1" t="s">
         <v>313</v>
       </c>
-      <c r="JK1" t="s">
+      <c r="JL1" t="s">
         <v>314</v>
       </c>
-      <c r="JL1" t="s">
+      <c r="JM1" t="s">
         <v>315</v>
       </c>
-      <c r="JM1" t="s">
+      <c r="JN1" t="s">
         <v>316</v>
       </c>
-      <c r="JN1" t="s">
+      <c r="JO1" t="s">
         <v>317</v>
       </c>
-      <c r="JO1" t="s">
+      <c r="JP1" t="s">
         <v>318</v>
       </c>
-      <c r="JP1" t="s">
+      <c r="JQ1" t="s">
         <v>319</v>
       </c>
-      <c r="JQ1" t="s">
+      <c r="JR1" t="s">
         <v>320</v>
       </c>
-      <c r="JR1" t="s">
+      <c r="JS1" t="s">
         <v>321</v>
       </c>
-      <c r="JS1" t="s">
+      <c r="JT1" t="s">
         <v>322</v>
       </c>
-      <c r="JT1" t="s">
+      <c r="JU1" t="s">
         <v>323</v>
       </c>
-      <c r="JU1" t="s">
+      <c r="JV1" t="s">
         <v>324</v>
       </c>
-      <c r="JV1" t="s">
+      <c r="JW1" t="s">
         <v>325</v>
       </c>
-      <c r="JW1" t="s">
+      <c r="JX1" t="s">
         <v>326</v>
       </c>
-      <c r="JX1" t="s">
+      <c r="JY1" t="s">
         <v>327</v>
       </c>
-      <c r="JY1" t="s">
+      <c r="JZ1" t="s">
         <v>328</v>
       </c>
-      <c r="JZ1" t="s">
+      <c r="KA1" t="s">
         <v>329</v>
       </c>
-      <c r="KA1" t="s">
+      <c r="KB1" t="s">
         <v>330</v>
       </c>
-      <c r="KB1" t="s">
+      <c r="KC1" t="s">
         <v>331</v>
       </c>
-      <c r="KC1" t="s">
+      <c r="KD1" t="s">
         <v>332</v>
       </c>
-      <c r="KD1" t="s">
+      <c r="KE1" t="s">
         <v>333</v>
       </c>
-      <c r="KE1" t="s">
+      <c r="KF1" t="s">
         <v>334</v>
       </c>
-      <c r="KF1" t="s">
+      <c r="KG1" t="s">
         <v>335</v>
       </c>
-      <c r="KG1" t="s">
+      <c r="KH1" t="s">
         <v>336</v>
       </c>
-      <c r="KH1" t="s">
+      <c r="KI1" t="s">
         <v>337</v>
       </c>
-      <c r="KI1" t="s">
+      <c r="KJ1" t="s">
         <v>338</v>
       </c>
-      <c r="KJ1" t="s">
+      <c r="KK1" t="s">
         <v>339</v>
       </c>
-      <c r="KK1" t="s">
+      <c r="KL1" t="s">
         <v>340</v>
       </c>
-      <c r="KL1" t="s">
+      <c r="KM1" t="s">
         <v>341</v>
       </c>
-      <c r="KM1" t="s">
+      <c r="KN1" t="s">
         <v>342</v>
       </c>
-      <c r="KN1" t="s">
+      <c r="KO1" t="s">
         <v>343</v>
       </c>
-      <c r="KO1" t="s">
+      <c r="KP1" t="s">
         <v>344</v>
       </c>
-      <c r="KP1" t="s">
+      <c r="KQ1" t="s">
         <v>345</v>
       </c>
-      <c r="KQ1" t="s">
+      <c r="KR1" t="s">
         <v>346</v>
       </c>
-      <c r="KR1" t="s">
+      <c r="KS1" t="s">
         <v>347</v>
       </c>
-      <c r="KS1" t="s">
+      <c r="KT1" t="s">
         <v>348</v>
       </c>
-      <c r="KT1" t="s">
+      <c r="KU1" t="s">
         <v>349</v>
       </c>
-      <c r="KU1" t="s">
+      <c r="KV1" t="s">
         <v>350</v>
       </c>
-      <c r="KV1" t="s">
+      <c r="KW1" t="s">
         <v>351</v>
       </c>
-      <c r="KW1" t="s">
+      <c r="KX1" t="s">
         <v>352</v>
       </c>
-      <c r="KX1" t="s">
+      <c r="KY1" t="s">
         <v>353</v>
       </c>
-      <c r="KY1" t="s">
+      <c r="KZ1" t="s">
         <v>354</v>
       </c>
-      <c r="KZ1" t="s">
+      <c r="LA1" t="s">
         <v>355</v>
       </c>
-      <c r="LA1" t="s">
+      <c r="LB1" t="s">
         <v>356</v>
       </c>
-      <c r="LB1" t="s">
+      <c r="LC1" t="s">
         <v>357</v>
       </c>
-      <c r="LC1" t="s">
+      <c r="LD1" t="s">
         <v>358</v>
       </c>
-      <c r="LD1" t="s">
+      <c r="LE1" t="s">
         <v>359</v>
       </c>
-      <c r="LE1" t="s">
+      <c r="LF1" t="s">
         <v>360</v>
       </c>
-      <c r="LF1" t="s">
+      <c r="LG1" t="s">
         <v>361</v>
       </c>
-      <c r="LG1" t="s">
+      <c r="LH1" t="s">
         <v>362</v>
       </c>
-      <c r="LH1" t="s">
+      <c r="LI1" t="s">
         <v>363</v>
       </c>
-      <c r="LI1" t="s">
+      <c r="LJ1" t="s">
         <v>364</v>
       </c>
-      <c r="LJ1" t="s">
+      <c r="LK1" t="s">
         <v>365</v>
       </c>
-      <c r="LK1" t="s">
+      <c r="LL1" t="s">
         <v>366</v>
       </c>
-      <c r="LL1" t="s">
+      <c r="LM1" t="s">
         <v>367</v>
       </c>
-      <c r="LM1" t="s">
+      <c r="LN1" t="s">
         <v>368</v>
       </c>
-      <c r="LN1" t="s">
+      <c r="LO1" t="s">
         <v>369</v>
       </c>
-      <c r="LO1" t="s">
+      <c r="LP1" t="s">
         <v>370</v>
       </c>
-      <c r="LP1" t="s">
+      <c r="LQ1" t="s">
         <v>371</v>
       </c>
-      <c r="LQ1" t="s">
+      <c r="LR1" t="s">
         <v>372</v>
       </c>
-      <c r="LR1" t="s">
+      <c r="LS1" t="s">
         <v>373</v>
       </c>
-      <c r="LS1" t="s">
+      <c r="LT1" t="s">
         <v>374</v>
       </c>
-      <c r="LT1" t="s">
+      <c r="LU1" t="s">
         <v>375</v>
       </c>
-      <c r="LU1" t="s">
+      <c r="LV1" t="s">
         <v>376</v>
       </c>
-      <c r="LV1" t="s">
+      <c r="LW1" t="s">
         <v>377</v>
       </c>
-      <c r="LW1" t="s">
+      <c r="LX1" t="s">
         <v>378</v>
       </c>
-      <c r="LX1" t="s">
+      <c r="LY1" t="s">
         <v>379</v>
       </c>
-      <c r="LY1" t="s">
+      <c r="LZ1" t="s">
         <v>380</v>
       </c>
-      <c r="LZ1" t="s">
+      <c r="MA1" t="s">
         <v>381</v>
       </c>
-      <c r="MA1" t="s">
+      <c r="MB1" t="s">
         <v>382</v>
       </c>
-      <c r="MB1" t="s">
+      <c r="MC1" t="s">
         <v>383</v>
       </c>
-      <c r="MC1" t="s">
+      <c r="MD1" t="s">
         <v>384</v>
       </c>
-      <c r="MD1" t="s">
+      <c r="ME1" t="s">
         <v>385</v>
       </c>
-      <c r="ME1" t="s">
+      <c r="MF1" t="s">
         <v>386</v>
       </c>
-      <c r="MF1" t="s">
+      <c r="MG1" t="s">
         <v>387</v>
       </c>
-      <c r="MG1" t="s">
+      <c r="MH1" t="s">
         <v>388</v>
       </c>
-      <c r="MH1" t="s">
+      <c r="MI1" t="s">
         <v>389</v>
       </c>
-      <c r="MI1" t="s">
+      <c r="MJ1" t="s">
         <v>390</v>
       </c>
-      <c r="MJ1" t="s">
+      <c r="MK1" t="s">
         <v>391</v>
       </c>
-      <c r="MK1" t="s">
+      <c r="ML1" t="s">
         <v>392</v>
       </c>
-      <c r="ML1" t="s">
+      <c r="MM1" t="s">
         <v>393</v>
       </c>
-      <c r="MM1" t="s">
+      <c r="MN1" t="s">
         <v>394</v>
       </c>
-      <c r="MN1" t="s">
+      <c r="MO1" t="s">
         <v>395</v>
       </c>
-      <c r="MO1" t="s">
+      <c r="MP1" t="s">
         <v>396</v>
       </c>
-      <c r="MP1" t="s">
+      <c r="MQ1" t="s">
         <v>397</v>
       </c>
-      <c r="MQ1" t="s">
+      <c r="MR1" t="s">
         <v>398</v>
       </c>
-      <c r="MR1" t="s">
+      <c r="MS1" t="s">
         <v>399</v>
       </c>
-      <c r="MS1" t="s">
+      <c r="MT1" t="s">
         <v>400</v>
       </c>
-      <c r="MT1" t="s">
+      <c r="MU1" t="s">
         <v>401</v>
       </c>
-      <c r="MU1" t="s">
+      <c r="MV1" t="s">
         <v>402</v>
       </c>
-      <c r="MV1" t="s">
+      <c r="MW1" t="s">
         <v>403</v>
       </c>
-      <c r="MW1" t="s">
+      <c r="MX1" t="s">
         <v>404</v>
       </c>
-      <c r="MX1" t="s">
+      <c r="MY1" t="s">
         <v>405</v>
       </c>
-      <c r="MY1" t="s">
+      <c r="MZ1" t="s">
         <v>70</v>
       </c>
-      <c r="MZ1" t="s">
+      <c r="NA1" t="s">
         <v>71</v>
       </c>
-      <c r="NA1" t="s">
+      <c r="NB1" t="s">
         <v>72</v>
       </c>
-      <c r="NB1" t="s">
+      <c r="NC1" t="s">
         <v>73</v>
       </c>
-      <c r="NC1" t="s">
+      <c r="ND1" t="s">
         <v>74</v>
       </c>
-      <c r="ND1" t="s">
+      <c r="NE1" t="s">
         <v>75</v>
       </c>
-      <c r="NE1" t="s">
+      <c r="NF1" t="s">
         <v>76</v>
       </c>
-      <c r="NF1" t="s">
+      <c r="NG1" t="s">
         <v>77</v>
       </c>
-      <c r="NG1" t="s">
+      <c r="NH1" t="s">
         <v>78</v>
       </c>
-      <c r="NH1" t="s">
+      <c r="NI1" t="s">
         <v>79</v>
       </c>
-      <c r="NI1" t="s">
+      <c r="NJ1" t="s">
         <v>80</v>
       </c>
-      <c r="NJ1" t="s">
+      <c r="NK1" t="s">
         <v>81</v>
       </c>
-      <c r="NK1" t="s">
+      <c r="NL1" t="s">
         <v>82</v>
       </c>
-      <c r="NL1" t="s">
+      <c r="NM1" t="s">
         <v>83</v>
       </c>
-      <c r="NM1" t="s">
+      <c r="NN1" t="s">
         <v>84</v>
       </c>
-      <c r="NN1" t="s">
+      <c r="NO1" t="s">
         <v>85</v>
       </c>
-      <c r="NO1" t="s">
+      <c r="NP1" t="s">
         <v>86</v>
       </c>
-      <c r="NP1" t="s">
+      <c r="NQ1" t="s">
         <v>87</v>
       </c>
-      <c r="NQ1" t="s">
+      <c r="NR1" t="s">
         <v>88</v>
       </c>
-      <c r="NR1" t="s">
+      <c r="NS1" t="s">
         <v>89</v>
       </c>
-      <c r="NS1" t="s">
+      <c r="NT1" t="s">
         <v>90</v>
       </c>
-      <c r="NT1" t="s">
+      <c r="NU1" t="s">
         <v>91</v>
       </c>
-      <c r="NU1" t="s">
+      <c r="NV1" t="s">
         <v>92</v>
       </c>
-      <c r="NV1" t="s">
+      <c r="NW1" t="s">
         <v>93</v>
       </c>
-      <c r="NW1" t="s">
+      <c r="NX1" t="s">
         <v>94</v>
       </c>
-      <c r="NX1" t="s">
+      <c r="NY1" t="s">
         <v>95</v>
       </c>
-      <c r="NY1" t="s">
+      <c r="NZ1" t="s">
         <v>96</v>
       </c>
-      <c r="NZ1" t="s">
+      <c r="OA1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:390" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:391" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -3092,23 +3098,23 @@
         <v>0</v>
       </c>
       <c r="AF2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG2" s="1">
         <v>-0.1</v>
       </c>
-      <c r="AG2" s="1">
-        <v>0</v>
-      </c>
       <c r="AH2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI2" s="1">
         <v>-0.1</v>
       </c>
-      <c r="AI2" s="1">
-        <v>0</v>
-      </c>
       <c r="AJ2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK2" s="1">
         <v>-32765</v>
       </c>
-      <c r="AK2" s="1">
-        <v>0</v>
-      </c>
       <c r="AL2" s="1">
         <v>0</v>
       </c>
@@ -3131,37 +3137,37 @@
         <v>0</v>
       </c>
       <c r="AS2" s="1">
-        <v>-127</v>
+        <v>0</v>
       </c>
       <c r="AT2" s="1">
         <v>-127</v>
       </c>
       <c r="AU2" s="1">
-        <v>0</v>
+        <v>-127</v>
       </c>
       <c r="AV2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AW2" s="1">
         <v>-127</v>
       </c>
-      <c r="AW2" s="1">
-        <v>0</v>
-      </c>
       <c r="AX2" s="1">
-        <v>-0.1</v>
+        <v>0</v>
       </c>
       <c r="AY2" s="1">
         <v>-0.1</v>
       </c>
       <c r="AZ2" s="1">
-        <v>0</v>
+        <v>-0.1</v>
       </c>
       <c r="BA2" s="1">
+        <v>0</v>
+      </c>
+      <c r="BB2" s="1">
         <v>-0.1</v>
       </c>
-      <c r="BB2" s="1">
-        <v>0</v>
-      </c>
       <c r="BC2" s="1">
-        <v>1.99</v>
+        <v>0</v>
       </c>
       <c r="BD2" s="1">
         <v>1.99</v>
@@ -3245,7 +3251,7 @@
         <v>1.99</v>
       </c>
       <c r="CE2" s="1">
-        <v>-128</v>
+        <v>1.99</v>
       </c>
       <c r="CF2" s="1">
         <v>-128</v>
@@ -3413,7 +3419,7 @@
         <v>-128</v>
       </c>
       <c r="EI2" s="1">
-        <v>-0.1</v>
+        <v>-128</v>
       </c>
       <c r="EJ2" s="1">
         <v>-0.1</v>
@@ -3496,8 +3502,8 @@
       <c r="FJ2" s="1">
         <v>-0.1</v>
       </c>
-      <c r="FK2">
-        <v>0</v>
+      <c r="FK2" s="1">
+        <v>-0.1</v>
       </c>
       <c r="FL2">
         <v>0</v>
@@ -4168,8 +4174,11 @@
       <c r="NZ2">
         <v>0</v>
       </c>
+      <c r="OA2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:390" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:391" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -4261,79 +4270,79 @@
         <v>1</v>
       </c>
       <c r="AE3">
+        <v>1</v>
+      </c>
+      <c r="AF3">
         <v>65535</v>
       </c>
-      <c r="AF3">
+      <c r="AG3">
         <v>25.5</v>
       </c>
-      <c r="AG3">
+      <c r="AH3">
         <v>255</v>
       </c>
-      <c r="AH3">
+      <c r="AI3">
         <v>25.5</v>
       </c>
-      <c r="AI3">
+      <c r="AJ3">
         <v>255</v>
       </c>
-      <c r="AJ3">
+      <c r="AK3">
         <v>32765</v>
-      </c>
-      <c r="AK3">
-        <v>65535</v>
       </c>
       <c r="AL3">
         <v>65535</v>
       </c>
       <c r="AM3">
-        <v>4294967295</v>
+        <v>65535</v>
       </c>
       <c r="AN3">
         <v>4294967295</v>
       </c>
       <c r="AO3">
+        <v>4294967295</v>
+      </c>
+      <c r="AP3">
         <v>100</v>
-      </c>
-      <c r="AP3">
-        <v>65535</v>
       </c>
       <c r="AQ3">
         <v>65535</v>
       </c>
       <c r="AR3">
+        <v>65535</v>
+      </c>
+      <c r="AS3">
         <v>100</v>
-      </c>
-      <c r="AS3">
-        <v>127</v>
       </c>
       <c r="AT3">
         <v>127</v>
       </c>
       <c r="AU3">
+        <v>127</v>
+      </c>
+      <c r="AV3">
         <v>255</v>
       </c>
-      <c r="AV3">
+      <c r="AW3">
         <v>127</v>
       </c>
-      <c r="AW3">
+      <c r="AX3">
         <v>255</v>
       </c>
-      <c r="AX3">
+      <c r="AY3">
         <v>6553.5</v>
       </c>
-      <c r="AY3">
+      <c r="AZ3">
         <v>25.5</v>
       </c>
-      <c r="AZ3">
+      <c r="BA3">
         <v>255</v>
       </c>
-      <c r="BA3">
+      <c r="BB3">
         <v>25.5</v>
       </c>
-      <c r="BB3">
+      <c r="BC3">
         <v>255</v>
-      </c>
-      <c r="BC3">
-        <v>4.55</v>
       </c>
       <c r="BD3">
         <v>4.55</v>
@@ -4417,7 +4426,7 @@
         <v>4.55</v>
       </c>
       <c r="CE3">
-        <v>127</v>
+        <v>4.55</v>
       </c>
       <c r="CF3">
         <v>127</v>
@@ -4585,7 +4594,7 @@
         <v>127</v>
       </c>
       <c r="EI3">
-        <v>25.5</v>
+        <v>127</v>
       </c>
       <c r="EJ3">
         <v>25.5</v>
@@ -4669,7 +4678,7 @@
         <v>25.5</v>
       </c>
       <c r="FK3">
-        <v>1</v>
+        <v>25.5</v>
       </c>
       <c r="FL3">
         <v>1</v>
@@ -5340,22 +5349,22 @@
       <c r="NZ3">
         <v>1</v>
       </c>
+      <c r="OA3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:390" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:391" x14ac:dyDescent="0.25">
       <c r="F4" t="s">
         <v>65</v>
       </c>
-      <c r="AE4" t="s">
-        <v>64</v>
-      </c>
       <c r="AF4" t="s">
         <v>64</v>
       </c>
-      <c r="AH4" t="s">
+      <c r="AG4" t="s">
         <v>64</v>
       </c>
-      <c r="AJ4" t="s">
-        <v>61</v>
+      <c r="AI4" t="s">
+        <v>64</v>
       </c>
       <c r="AK4" t="s">
         <v>61</v>
@@ -5364,43 +5373,43 @@
         <v>61</v>
       </c>
       <c r="AM4" t="s">
+        <v>61</v>
+      </c>
+      <c r="AN4" t="s">
         <v>62</v>
       </c>
-      <c r="AN4" t="s">
+      <c r="AO4" t="s">
         <v>63</v>
       </c>
-      <c r="AO4" t="s">
+      <c r="AP4" t="s">
         <v>66</v>
-      </c>
-      <c r="AP4" t="s">
-        <v>67</v>
       </c>
       <c r="AQ4" t="s">
         <v>67</v>
       </c>
       <c r="AR4" t="s">
+        <v>67</v>
+      </c>
+      <c r="AS4" t="s">
         <v>66</v>
-      </c>
-      <c r="AS4" t="s">
-        <v>68</v>
       </c>
       <c r="AT4" t="s">
         <v>68</v>
       </c>
-      <c r="AV4" t="s">
+      <c r="AU4" t="s">
         <v>68</v>
       </c>
-      <c r="AX4" t="s">
-        <v>69</v>
+      <c r="AW4" t="s">
+        <v>68</v>
       </c>
       <c r="AY4" t="s">
         <v>69</v>
       </c>
-      <c r="BA4" t="s">
+      <c r="AZ4" t="s">
         <v>69</v>
       </c>
-      <c r="BC4" t="s">
-        <v>64</v>
+      <c r="BB4" t="s">
+        <v>69</v>
       </c>
       <c r="BD4" t="s">
         <v>64</v>
@@ -5484,7 +5493,7 @@
         <v>64</v>
       </c>
       <c r="CE4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="CF4" t="s">
         <v>68</v>
@@ -5652,7 +5661,7 @@
         <v>68</v>
       </c>
       <c r="EI4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="EJ4" t="s">
         <v>69</v>
@@ -5734,6 +5743,1574 @@
       </c>
       <c r="FJ4" t="s">
         <v>69</v>
+      </c>
+      <c r="FK4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:391" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <f>A5+1</f>
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:BO5" si="0">B5+1</f>
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="R5">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="S5">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="U5">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="V5">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="W5">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="X5">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="Y5">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="Z5">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="AA5">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="AB5">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="AC5">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="AD5">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="AE5">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="AF5">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="AG5">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="AH5">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="AI5">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="AJ5">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="AK5">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="AL5">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="AM5">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="AN5">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="AO5">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="AP5">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="AQ5">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="AR5">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="AS5">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="AT5">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="AU5">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="AV5">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="AW5">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="AX5">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="AY5">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="AZ5">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="BA5">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="BB5">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="BC5">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="BD5">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="BE5">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="BF5">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="BG5">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="BH5">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="BI5">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="BJ5">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="BK5">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+      <c r="BL5">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="BM5">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="BN5">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="BO5">
+        <f t="shared" si="0"/>
+        <v>66</v>
+      </c>
+      <c r="BP5">
+        <f t="shared" ref="BP5:EA5" si="1">BO5+1</f>
+        <v>67</v>
+      </c>
+      <c r="BQ5">
+        <f t="shared" si="1"/>
+        <v>68</v>
+      </c>
+      <c r="BR5">
+        <f t="shared" si="1"/>
+        <v>69</v>
+      </c>
+      <c r="BS5">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+      <c r="BT5">
+        <f t="shared" si="1"/>
+        <v>71</v>
+      </c>
+      <c r="BU5">
+        <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
+      <c r="BV5">
+        <f t="shared" si="1"/>
+        <v>73</v>
+      </c>
+      <c r="BW5">
+        <f t="shared" si="1"/>
+        <v>74</v>
+      </c>
+      <c r="BX5">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+      <c r="BY5">
+        <f t="shared" si="1"/>
+        <v>76</v>
+      </c>
+      <c r="BZ5">
+        <f t="shared" si="1"/>
+        <v>77</v>
+      </c>
+      <c r="CA5">
+        <f t="shared" si="1"/>
+        <v>78</v>
+      </c>
+      <c r="CB5">
+        <f t="shared" si="1"/>
+        <v>79</v>
+      </c>
+      <c r="CC5">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="CD5">
+        <f t="shared" si="1"/>
+        <v>81</v>
+      </c>
+      <c r="CE5">
+        <f t="shared" si="1"/>
+        <v>82</v>
+      </c>
+      <c r="CF5">
+        <f t="shared" si="1"/>
+        <v>83</v>
+      </c>
+      <c r="CG5">
+        <f t="shared" si="1"/>
+        <v>84</v>
+      </c>
+      <c r="CH5">
+        <f t="shared" si="1"/>
+        <v>85</v>
+      </c>
+      <c r="CI5">
+        <f t="shared" si="1"/>
+        <v>86</v>
+      </c>
+      <c r="CJ5">
+        <f t="shared" si="1"/>
+        <v>87</v>
+      </c>
+      <c r="CK5">
+        <f t="shared" si="1"/>
+        <v>88</v>
+      </c>
+      <c r="CL5">
+        <f t="shared" si="1"/>
+        <v>89</v>
+      </c>
+      <c r="CM5">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+      <c r="CN5">
+        <f t="shared" si="1"/>
+        <v>91</v>
+      </c>
+      <c r="CO5">
+        <f t="shared" si="1"/>
+        <v>92</v>
+      </c>
+      <c r="CP5">
+        <f t="shared" si="1"/>
+        <v>93</v>
+      </c>
+      <c r="CQ5">
+        <f t="shared" si="1"/>
+        <v>94</v>
+      </c>
+      <c r="CR5">
+        <f t="shared" si="1"/>
+        <v>95</v>
+      </c>
+      <c r="CS5">
+        <f t="shared" si="1"/>
+        <v>96</v>
+      </c>
+      <c r="CT5">
+        <f t="shared" si="1"/>
+        <v>97</v>
+      </c>
+      <c r="CU5">
+        <f t="shared" si="1"/>
+        <v>98</v>
+      </c>
+      <c r="CV5">
+        <f t="shared" si="1"/>
+        <v>99</v>
+      </c>
+      <c r="CW5">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="CX5">
+        <f t="shared" si="1"/>
+        <v>101</v>
+      </c>
+      <c r="CY5">
+        <f t="shared" si="1"/>
+        <v>102</v>
+      </c>
+      <c r="CZ5">
+        <f t="shared" si="1"/>
+        <v>103</v>
+      </c>
+      <c r="DA5">
+        <f t="shared" si="1"/>
+        <v>104</v>
+      </c>
+      <c r="DB5">
+        <f t="shared" si="1"/>
+        <v>105</v>
+      </c>
+      <c r="DC5">
+        <f t="shared" si="1"/>
+        <v>106</v>
+      </c>
+      <c r="DD5">
+        <f t="shared" si="1"/>
+        <v>107</v>
+      </c>
+      <c r="DE5">
+        <f t="shared" si="1"/>
+        <v>108</v>
+      </c>
+      <c r="DF5">
+        <f t="shared" si="1"/>
+        <v>109</v>
+      </c>
+      <c r="DG5">
+        <f t="shared" si="1"/>
+        <v>110</v>
+      </c>
+      <c r="DH5">
+        <f t="shared" si="1"/>
+        <v>111</v>
+      </c>
+      <c r="DI5">
+        <f t="shared" si="1"/>
+        <v>112</v>
+      </c>
+      <c r="DJ5">
+        <f t="shared" si="1"/>
+        <v>113</v>
+      </c>
+      <c r="DK5">
+        <f t="shared" si="1"/>
+        <v>114</v>
+      </c>
+      <c r="DL5">
+        <f t="shared" si="1"/>
+        <v>115</v>
+      </c>
+      <c r="DM5">
+        <f t="shared" si="1"/>
+        <v>116</v>
+      </c>
+      <c r="DN5">
+        <f t="shared" si="1"/>
+        <v>117</v>
+      </c>
+      <c r="DO5">
+        <f t="shared" si="1"/>
+        <v>118</v>
+      </c>
+      <c r="DP5">
+        <f t="shared" si="1"/>
+        <v>119</v>
+      </c>
+      <c r="DQ5">
+        <f t="shared" si="1"/>
+        <v>120</v>
+      </c>
+      <c r="DR5">
+        <f t="shared" si="1"/>
+        <v>121</v>
+      </c>
+      <c r="DS5">
+        <f t="shared" si="1"/>
+        <v>122</v>
+      </c>
+      <c r="DT5">
+        <f t="shared" si="1"/>
+        <v>123</v>
+      </c>
+      <c r="DU5">
+        <f t="shared" si="1"/>
+        <v>124</v>
+      </c>
+      <c r="DV5">
+        <f t="shared" si="1"/>
+        <v>125</v>
+      </c>
+      <c r="DW5">
+        <f t="shared" si="1"/>
+        <v>126</v>
+      </c>
+      <c r="DX5">
+        <f t="shared" si="1"/>
+        <v>127</v>
+      </c>
+      <c r="DY5">
+        <f t="shared" si="1"/>
+        <v>128</v>
+      </c>
+      <c r="DZ5">
+        <f t="shared" si="1"/>
+        <v>129</v>
+      </c>
+      <c r="EA5">
+        <f t="shared" si="1"/>
+        <v>130</v>
+      </c>
+      <c r="EB5">
+        <f t="shared" ref="EB5:GM5" si="2">EA5+1</f>
+        <v>131</v>
+      </c>
+      <c r="EC5">
+        <f t="shared" si="2"/>
+        <v>132</v>
+      </c>
+      <c r="ED5">
+        <f t="shared" si="2"/>
+        <v>133</v>
+      </c>
+      <c r="EE5">
+        <f t="shared" si="2"/>
+        <v>134</v>
+      </c>
+      <c r="EF5">
+        <f t="shared" si="2"/>
+        <v>135</v>
+      </c>
+      <c r="EG5">
+        <f t="shared" si="2"/>
+        <v>136</v>
+      </c>
+      <c r="EH5">
+        <f t="shared" si="2"/>
+        <v>137</v>
+      </c>
+      <c r="EI5">
+        <f t="shared" si="2"/>
+        <v>138</v>
+      </c>
+      <c r="EJ5">
+        <f t="shared" si="2"/>
+        <v>139</v>
+      </c>
+      <c r="EK5">
+        <f t="shared" si="2"/>
+        <v>140</v>
+      </c>
+      <c r="EL5">
+        <f t="shared" si="2"/>
+        <v>141</v>
+      </c>
+      <c r="EM5">
+        <f t="shared" si="2"/>
+        <v>142</v>
+      </c>
+      <c r="EN5">
+        <f t="shared" si="2"/>
+        <v>143</v>
+      </c>
+      <c r="EO5">
+        <f t="shared" si="2"/>
+        <v>144</v>
+      </c>
+      <c r="EP5">
+        <f t="shared" si="2"/>
+        <v>145</v>
+      </c>
+      <c r="EQ5">
+        <f t="shared" si="2"/>
+        <v>146</v>
+      </c>
+      <c r="ER5">
+        <f t="shared" si="2"/>
+        <v>147</v>
+      </c>
+      <c r="ES5">
+        <f t="shared" si="2"/>
+        <v>148</v>
+      </c>
+      <c r="ET5">
+        <f t="shared" si="2"/>
+        <v>149</v>
+      </c>
+      <c r="EU5">
+        <f t="shared" si="2"/>
+        <v>150</v>
+      </c>
+      <c r="EV5">
+        <f t="shared" si="2"/>
+        <v>151</v>
+      </c>
+      <c r="EW5">
+        <f t="shared" si="2"/>
+        <v>152</v>
+      </c>
+      <c r="EX5">
+        <f t="shared" si="2"/>
+        <v>153</v>
+      </c>
+      <c r="EY5">
+        <f t="shared" si="2"/>
+        <v>154</v>
+      </c>
+      <c r="EZ5">
+        <f t="shared" si="2"/>
+        <v>155</v>
+      </c>
+      <c r="FA5">
+        <f t="shared" si="2"/>
+        <v>156</v>
+      </c>
+      <c r="FB5">
+        <f t="shared" si="2"/>
+        <v>157</v>
+      </c>
+      <c r="FC5">
+        <f t="shared" si="2"/>
+        <v>158</v>
+      </c>
+      <c r="FD5">
+        <f t="shared" si="2"/>
+        <v>159</v>
+      </c>
+      <c r="FE5">
+        <f t="shared" si="2"/>
+        <v>160</v>
+      </c>
+      <c r="FF5">
+        <f t="shared" si="2"/>
+        <v>161</v>
+      </c>
+      <c r="FG5">
+        <f t="shared" si="2"/>
+        <v>162</v>
+      </c>
+      <c r="FH5">
+        <f t="shared" si="2"/>
+        <v>163</v>
+      </c>
+      <c r="FI5">
+        <f t="shared" si="2"/>
+        <v>164</v>
+      </c>
+      <c r="FJ5">
+        <f t="shared" si="2"/>
+        <v>165</v>
+      </c>
+      <c r="FK5">
+        <f t="shared" si="2"/>
+        <v>166</v>
+      </c>
+      <c r="FL5">
+        <f t="shared" si="2"/>
+        <v>167</v>
+      </c>
+      <c r="FM5">
+        <f t="shared" si="2"/>
+        <v>168</v>
+      </c>
+      <c r="FN5">
+        <f t="shared" si="2"/>
+        <v>169</v>
+      </c>
+      <c r="FO5">
+        <f t="shared" si="2"/>
+        <v>170</v>
+      </c>
+      <c r="FP5">
+        <f t="shared" si="2"/>
+        <v>171</v>
+      </c>
+      <c r="FQ5">
+        <f t="shared" si="2"/>
+        <v>172</v>
+      </c>
+      <c r="FR5">
+        <f t="shared" si="2"/>
+        <v>173</v>
+      </c>
+      <c r="FS5">
+        <f t="shared" si="2"/>
+        <v>174</v>
+      </c>
+      <c r="FT5">
+        <f t="shared" si="2"/>
+        <v>175</v>
+      </c>
+      <c r="FU5">
+        <f t="shared" si="2"/>
+        <v>176</v>
+      </c>
+      <c r="FV5">
+        <f t="shared" si="2"/>
+        <v>177</v>
+      </c>
+      <c r="FW5">
+        <f t="shared" si="2"/>
+        <v>178</v>
+      </c>
+      <c r="FX5">
+        <f t="shared" si="2"/>
+        <v>179</v>
+      </c>
+      <c r="FY5">
+        <f t="shared" si="2"/>
+        <v>180</v>
+      </c>
+      <c r="FZ5">
+        <f t="shared" si="2"/>
+        <v>181</v>
+      </c>
+      <c r="GA5">
+        <f t="shared" si="2"/>
+        <v>182</v>
+      </c>
+      <c r="GB5">
+        <f t="shared" si="2"/>
+        <v>183</v>
+      </c>
+      <c r="GC5">
+        <f t="shared" si="2"/>
+        <v>184</v>
+      </c>
+      <c r="GD5">
+        <f t="shared" si="2"/>
+        <v>185</v>
+      </c>
+      <c r="GE5">
+        <f t="shared" si="2"/>
+        <v>186</v>
+      </c>
+      <c r="GF5">
+        <f t="shared" si="2"/>
+        <v>187</v>
+      </c>
+      <c r="GG5">
+        <f t="shared" si="2"/>
+        <v>188</v>
+      </c>
+      <c r="GH5">
+        <f t="shared" si="2"/>
+        <v>189</v>
+      </c>
+      <c r="GI5">
+        <f t="shared" si="2"/>
+        <v>190</v>
+      </c>
+      <c r="GJ5">
+        <f t="shared" si="2"/>
+        <v>191</v>
+      </c>
+      <c r="GK5">
+        <f t="shared" si="2"/>
+        <v>192</v>
+      </c>
+      <c r="GL5">
+        <f t="shared" si="2"/>
+        <v>193</v>
+      </c>
+      <c r="GM5">
+        <f t="shared" si="2"/>
+        <v>194</v>
+      </c>
+      <c r="GN5">
+        <f t="shared" ref="GN5:IY5" si="3">GM5+1</f>
+        <v>195</v>
+      </c>
+      <c r="GO5">
+        <f t="shared" si="3"/>
+        <v>196</v>
+      </c>
+      <c r="GP5">
+        <f t="shared" si="3"/>
+        <v>197</v>
+      </c>
+      <c r="GQ5">
+        <f t="shared" si="3"/>
+        <v>198</v>
+      </c>
+      <c r="GR5">
+        <f t="shared" si="3"/>
+        <v>199</v>
+      </c>
+      <c r="GS5">
+        <f t="shared" si="3"/>
+        <v>200</v>
+      </c>
+      <c r="GT5">
+        <f t="shared" si="3"/>
+        <v>201</v>
+      </c>
+      <c r="GU5">
+        <f t="shared" si="3"/>
+        <v>202</v>
+      </c>
+      <c r="GV5">
+        <f t="shared" si="3"/>
+        <v>203</v>
+      </c>
+      <c r="GW5">
+        <f t="shared" si="3"/>
+        <v>204</v>
+      </c>
+      <c r="GX5">
+        <f t="shared" si="3"/>
+        <v>205</v>
+      </c>
+      <c r="GY5">
+        <f t="shared" si="3"/>
+        <v>206</v>
+      </c>
+      <c r="GZ5">
+        <f t="shared" si="3"/>
+        <v>207</v>
+      </c>
+      <c r="HA5">
+        <f t="shared" si="3"/>
+        <v>208</v>
+      </c>
+      <c r="HB5">
+        <f t="shared" si="3"/>
+        <v>209</v>
+      </c>
+      <c r="HC5">
+        <f t="shared" si="3"/>
+        <v>210</v>
+      </c>
+      <c r="HD5">
+        <f t="shared" si="3"/>
+        <v>211</v>
+      </c>
+      <c r="HE5">
+        <f t="shared" si="3"/>
+        <v>212</v>
+      </c>
+      <c r="HF5">
+        <f t="shared" si="3"/>
+        <v>213</v>
+      </c>
+      <c r="HG5">
+        <f t="shared" si="3"/>
+        <v>214</v>
+      </c>
+      <c r="HH5">
+        <f t="shared" si="3"/>
+        <v>215</v>
+      </c>
+      <c r="HI5">
+        <f t="shared" si="3"/>
+        <v>216</v>
+      </c>
+      <c r="HJ5">
+        <f t="shared" si="3"/>
+        <v>217</v>
+      </c>
+      <c r="HK5">
+        <f t="shared" si="3"/>
+        <v>218</v>
+      </c>
+      <c r="HL5">
+        <f t="shared" si="3"/>
+        <v>219</v>
+      </c>
+      <c r="HM5">
+        <f t="shared" si="3"/>
+        <v>220</v>
+      </c>
+      <c r="HN5">
+        <f t="shared" si="3"/>
+        <v>221</v>
+      </c>
+      <c r="HO5">
+        <f t="shared" si="3"/>
+        <v>222</v>
+      </c>
+      <c r="HP5">
+        <f t="shared" si="3"/>
+        <v>223</v>
+      </c>
+      <c r="HQ5">
+        <f t="shared" si="3"/>
+        <v>224</v>
+      </c>
+      <c r="HR5">
+        <f t="shared" si="3"/>
+        <v>225</v>
+      </c>
+      <c r="HS5">
+        <f t="shared" si="3"/>
+        <v>226</v>
+      </c>
+      <c r="HT5">
+        <f t="shared" si="3"/>
+        <v>227</v>
+      </c>
+      <c r="HU5">
+        <f t="shared" si="3"/>
+        <v>228</v>
+      </c>
+      <c r="HV5">
+        <f t="shared" si="3"/>
+        <v>229</v>
+      </c>
+      <c r="HW5">
+        <f t="shared" si="3"/>
+        <v>230</v>
+      </c>
+      <c r="HX5">
+        <f t="shared" si="3"/>
+        <v>231</v>
+      </c>
+      <c r="HY5">
+        <f t="shared" si="3"/>
+        <v>232</v>
+      </c>
+      <c r="HZ5">
+        <f t="shared" si="3"/>
+        <v>233</v>
+      </c>
+      <c r="IA5">
+        <f t="shared" si="3"/>
+        <v>234</v>
+      </c>
+      <c r="IB5">
+        <f t="shared" si="3"/>
+        <v>235</v>
+      </c>
+      <c r="IC5">
+        <f t="shared" si="3"/>
+        <v>236</v>
+      </c>
+      <c r="ID5">
+        <f t="shared" si="3"/>
+        <v>237</v>
+      </c>
+      <c r="IE5">
+        <f t="shared" si="3"/>
+        <v>238</v>
+      </c>
+      <c r="IF5">
+        <f t="shared" si="3"/>
+        <v>239</v>
+      </c>
+      <c r="IG5">
+        <f t="shared" si="3"/>
+        <v>240</v>
+      </c>
+      <c r="IH5">
+        <f t="shared" si="3"/>
+        <v>241</v>
+      </c>
+      <c r="II5">
+        <f t="shared" si="3"/>
+        <v>242</v>
+      </c>
+      <c r="IJ5">
+        <f t="shared" si="3"/>
+        <v>243</v>
+      </c>
+      <c r="IK5">
+        <f t="shared" si="3"/>
+        <v>244</v>
+      </c>
+      <c r="IL5">
+        <f t="shared" si="3"/>
+        <v>245</v>
+      </c>
+      <c r="IM5">
+        <f t="shared" si="3"/>
+        <v>246</v>
+      </c>
+      <c r="IN5">
+        <f t="shared" si="3"/>
+        <v>247</v>
+      </c>
+      <c r="IO5">
+        <f t="shared" si="3"/>
+        <v>248</v>
+      </c>
+      <c r="IP5">
+        <f t="shared" si="3"/>
+        <v>249</v>
+      </c>
+      <c r="IQ5">
+        <f t="shared" si="3"/>
+        <v>250</v>
+      </c>
+      <c r="IR5">
+        <f t="shared" si="3"/>
+        <v>251</v>
+      </c>
+      <c r="IS5">
+        <f t="shared" si="3"/>
+        <v>252</v>
+      </c>
+      <c r="IT5">
+        <f t="shared" si="3"/>
+        <v>253</v>
+      </c>
+      <c r="IU5">
+        <f t="shared" si="3"/>
+        <v>254</v>
+      </c>
+      <c r="IV5">
+        <f t="shared" si="3"/>
+        <v>255</v>
+      </c>
+      <c r="IW5">
+        <f t="shared" si="3"/>
+        <v>256</v>
+      </c>
+      <c r="IX5">
+        <f t="shared" si="3"/>
+        <v>257</v>
+      </c>
+      <c r="IY5">
+        <f t="shared" si="3"/>
+        <v>258</v>
+      </c>
+      <c r="IZ5">
+        <f t="shared" ref="IZ5:LK5" si="4">IY5+1</f>
+        <v>259</v>
+      </c>
+      <c r="JA5">
+        <f t="shared" si="4"/>
+        <v>260</v>
+      </c>
+      <c r="JB5">
+        <f t="shared" si="4"/>
+        <v>261</v>
+      </c>
+      <c r="JC5">
+        <f t="shared" si="4"/>
+        <v>262</v>
+      </c>
+      <c r="JD5">
+        <f t="shared" si="4"/>
+        <v>263</v>
+      </c>
+      <c r="JE5">
+        <f t="shared" si="4"/>
+        <v>264</v>
+      </c>
+      <c r="JF5">
+        <f t="shared" si="4"/>
+        <v>265</v>
+      </c>
+      <c r="JG5">
+        <f t="shared" si="4"/>
+        <v>266</v>
+      </c>
+      <c r="JH5">
+        <f t="shared" si="4"/>
+        <v>267</v>
+      </c>
+      <c r="JI5">
+        <f t="shared" si="4"/>
+        <v>268</v>
+      </c>
+      <c r="JJ5">
+        <f t="shared" si="4"/>
+        <v>269</v>
+      </c>
+      <c r="JK5">
+        <f t="shared" si="4"/>
+        <v>270</v>
+      </c>
+      <c r="JL5">
+        <f t="shared" si="4"/>
+        <v>271</v>
+      </c>
+      <c r="JM5">
+        <f t="shared" si="4"/>
+        <v>272</v>
+      </c>
+      <c r="JN5">
+        <f t="shared" si="4"/>
+        <v>273</v>
+      </c>
+      <c r="JO5">
+        <f t="shared" si="4"/>
+        <v>274</v>
+      </c>
+      <c r="JP5">
+        <f t="shared" si="4"/>
+        <v>275</v>
+      </c>
+      <c r="JQ5">
+        <f t="shared" si="4"/>
+        <v>276</v>
+      </c>
+      <c r="JR5">
+        <f t="shared" si="4"/>
+        <v>277</v>
+      </c>
+      <c r="JS5">
+        <f t="shared" si="4"/>
+        <v>278</v>
+      </c>
+      <c r="JT5">
+        <f>JS5+1</f>
+        <v>279</v>
+      </c>
+      <c r="JU5">
+        <f t="shared" si="4"/>
+        <v>280</v>
+      </c>
+      <c r="JV5">
+        <f t="shared" si="4"/>
+        <v>281</v>
+      </c>
+      <c r="JW5">
+        <f t="shared" si="4"/>
+        <v>282</v>
+      </c>
+      <c r="JX5">
+        <f t="shared" si="4"/>
+        <v>283</v>
+      </c>
+      <c r="JY5">
+        <f t="shared" si="4"/>
+        <v>284</v>
+      </c>
+      <c r="JZ5">
+        <f t="shared" si="4"/>
+        <v>285</v>
+      </c>
+      <c r="KA5">
+        <f t="shared" si="4"/>
+        <v>286</v>
+      </c>
+      <c r="KB5">
+        <f t="shared" si="4"/>
+        <v>287</v>
+      </c>
+      <c r="KC5">
+        <f t="shared" si="4"/>
+        <v>288</v>
+      </c>
+      <c r="KD5">
+        <f t="shared" si="4"/>
+        <v>289</v>
+      </c>
+      <c r="KE5">
+        <f t="shared" si="4"/>
+        <v>290</v>
+      </c>
+      <c r="KF5">
+        <f t="shared" si="4"/>
+        <v>291</v>
+      </c>
+      <c r="KG5">
+        <f t="shared" si="4"/>
+        <v>292</v>
+      </c>
+      <c r="KH5">
+        <f t="shared" si="4"/>
+        <v>293</v>
+      </c>
+      <c r="KI5">
+        <f t="shared" si="4"/>
+        <v>294</v>
+      </c>
+      <c r="KJ5">
+        <f t="shared" si="4"/>
+        <v>295</v>
+      </c>
+      <c r="KK5">
+        <f t="shared" si="4"/>
+        <v>296</v>
+      </c>
+      <c r="KL5">
+        <f t="shared" si="4"/>
+        <v>297</v>
+      </c>
+      <c r="KM5">
+        <f t="shared" si="4"/>
+        <v>298</v>
+      </c>
+      <c r="KN5">
+        <f t="shared" si="4"/>
+        <v>299</v>
+      </c>
+      <c r="KO5">
+        <f t="shared" si="4"/>
+        <v>300</v>
+      </c>
+      <c r="KP5">
+        <f t="shared" si="4"/>
+        <v>301</v>
+      </c>
+      <c r="KQ5">
+        <f t="shared" si="4"/>
+        <v>302</v>
+      </c>
+      <c r="KR5">
+        <f t="shared" si="4"/>
+        <v>303</v>
+      </c>
+      <c r="KS5">
+        <f t="shared" si="4"/>
+        <v>304</v>
+      </c>
+      <c r="KT5">
+        <f t="shared" si="4"/>
+        <v>305</v>
+      </c>
+      <c r="KU5">
+        <f t="shared" si="4"/>
+        <v>306</v>
+      </c>
+      <c r="KV5">
+        <f t="shared" si="4"/>
+        <v>307</v>
+      </c>
+      <c r="KW5">
+        <f t="shared" si="4"/>
+        <v>308</v>
+      </c>
+      <c r="KX5">
+        <f t="shared" si="4"/>
+        <v>309</v>
+      </c>
+      <c r="KY5">
+        <f t="shared" si="4"/>
+        <v>310</v>
+      </c>
+      <c r="KZ5">
+        <f t="shared" si="4"/>
+        <v>311</v>
+      </c>
+      <c r="LA5">
+        <f t="shared" si="4"/>
+        <v>312</v>
+      </c>
+      <c r="LB5">
+        <f t="shared" si="4"/>
+        <v>313</v>
+      </c>
+      <c r="LC5">
+        <f t="shared" si="4"/>
+        <v>314</v>
+      </c>
+      <c r="LD5">
+        <f t="shared" si="4"/>
+        <v>315</v>
+      </c>
+      <c r="LE5">
+        <f t="shared" si="4"/>
+        <v>316</v>
+      </c>
+      <c r="LF5">
+        <f t="shared" si="4"/>
+        <v>317</v>
+      </c>
+      <c r="LG5">
+        <f t="shared" si="4"/>
+        <v>318</v>
+      </c>
+      <c r="LH5">
+        <f t="shared" si="4"/>
+        <v>319</v>
+      </c>
+      <c r="LI5">
+        <f t="shared" si="4"/>
+        <v>320</v>
+      </c>
+      <c r="LJ5">
+        <f t="shared" si="4"/>
+        <v>321</v>
+      </c>
+      <c r="LK5">
+        <f t="shared" si="4"/>
+        <v>322</v>
+      </c>
+      <c r="LL5">
+        <f t="shared" ref="LL5:NW5" si="5">LK5+1</f>
+        <v>323</v>
+      </c>
+      <c r="LM5">
+        <f t="shared" si="5"/>
+        <v>324</v>
+      </c>
+      <c r="LN5">
+        <f t="shared" si="5"/>
+        <v>325</v>
+      </c>
+      <c r="LO5">
+        <f t="shared" si="5"/>
+        <v>326</v>
+      </c>
+      <c r="LP5">
+        <f t="shared" si="5"/>
+        <v>327</v>
+      </c>
+      <c r="LQ5">
+        <f t="shared" si="5"/>
+        <v>328</v>
+      </c>
+      <c r="LR5">
+        <f t="shared" si="5"/>
+        <v>329</v>
+      </c>
+      <c r="LS5">
+        <f t="shared" si="5"/>
+        <v>330</v>
+      </c>
+      <c r="LT5">
+        <f t="shared" si="5"/>
+        <v>331</v>
+      </c>
+      <c r="LU5">
+        <f t="shared" si="5"/>
+        <v>332</v>
+      </c>
+      <c r="LV5">
+        <f t="shared" si="5"/>
+        <v>333</v>
+      </c>
+      <c r="LW5">
+        <f t="shared" si="5"/>
+        <v>334</v>
+      </c>
+      <c r="LX5">
+        <f t="shared" si="5"/>
+        <v>335</v>
+      </c>
+      <c r="LY5">
+        <f t="shared" si="5"/>
+        <v>336</v>
+      </c>
+      <c r="LZ5">
+        <f t="shared" si="5"/>
+        <v>337</v>
+      </c>
+      <c r="MA5">
+        <f t="shared" si="5"/>
+        <v>338</v>
+      </c>
+      <c r="MB5">
+        <f t="shared" si="5"/>
+        <v>339</v>
+      </c>
+      <c r="MC5">
+        <f t="shared" si="5"/>
+        <v>340</v>
+      </c>
+      <c r="MD5">
+        <f t="shared" si="5"/>
+        <v>341</v>
+      </c>
+      <c r="ME5">
+        <f t="shared" si="5"/>
+        <v>342</v>
+      </c>
+      <c r="MF5">
+        <f t="shared" si="5"/>
+        <v>343</v>
+      </c>
+      <c r="MG5">
+        <f t="shared" si="5"/>
+        <v>344</v>
+      </c>
+      <c r="MH5">
+        <f t="shared" si="5"/>
+        <v>345</v>
+      </c>
+      <c r="MI5">
+        <f t="shared" si="5"/>
+        <v>346</v>
+      </c>
+      <c r="MJ5">
+        <f t="shared" si="5"/>
+        <v>347</v>
+      </c>
+      <c r="MK5">
+        <f t="shared" si="5"/>
+        <v>348</v>
+      </c>
+      <c r="ML5">
+        <f t="shared" si="5"/>
+        <v>349</v>
+      </c>
+      <c r="MM5">
+        <f t="shared" si="5"/>
+        <v>350</v>
+      </c>
+      <c r="MN5">
+        <f t="shared" si="5"/>
+        <v>351</v>
+      </c>
+      <c r="MO5">
+        <f t="shared" si="5"/>
+        <v>352</v>
+      </c>
+      <c r="MP5">
+        <f t="shared" si="5"/>
+        <v>353</v>
+      </c>
+      <c r="MQ5">
+        <f t="shared" si="5"/>
+        <v>354</v>
+      </c>
+      <c r="MR5">
+        <f t="shared" si="5"/>
+        <v>355</v>
+      </c>
+      <c r="MS5">
+        <f t="shared" si="5"/>
+        <v>356</v>
+      </c>
+      <c r="MT5">
+        <f t="shared" si="5"/>
+        <v>357</v>
+      </c>
+      <c r="MU5">
+        <f t="shared" si="5"/>
+        <v>358</v>
+      </c>
+      <c r="MV5">
+        <f t="shared" si="5"/>
+        <v>359</v>
+      </c>
+      <c r="MW5">
+        <f t="shared" si="5"/>
+        <v>360</v>
+      </c>
+      <c r="MX5">
+        <f t="shared" si="5"/>
+        <v>361</v>
+      </c>
+      <c r="MY5">
+        <f t="shared" si="5"/>
+        <v>362</v>
+      </c>
+      <c r="MZ5">
+        <f t="shared" si="5"/>
+        <v>363</v>
+      </c>
+      <c r="NA5">
+        <f t="shared" si="5"/>
+        <v>364</v>
+      </c>
+      <c r="NB5">
+        <f t="shared" si="5"/>
+        <v>365</v>
+      </c>
+      <c r="NC5">
+        <f t="shared" si="5"/>
+        <v>366</v>
+      </c>
+      <c r="ND5">
+        <f t="shared" si="5"/>
+        <v>367</v>
+      </c>
+      <c r="NE5">
+        <f t="shared" si="5"/>
+        <v>368</v>
+      </c>
+      <c r="NF5">
+        <f t="shared" si="5"/>
+        <v>369</v>
+      </c>
+      <c r="NG5">
+        <f t="shared" si="5"/>
+        <v>370</v>
+      </c>
+      <c r="NH5">
+        <f t="shared" si="5"/>
+        <v>371</v>
+      </c>
+      <c r="NI5">
+        <f t="shared" si="5"/>
+        <v>372</v>
+      </c>
+      <c r="NJ5">
+        <f t="shared" si="5"/>
+        <v>373</v>
+      </c>
+      <c r="NK5">
+        <f t="shared" si="5"/>
+        <v>374</v>
+      </c>
+      <c r="NL5">
+        <f t="shared" si="5"/>
+        <v>375</v>
+      </c>
+      <c r="NM5">
+        <f t="shared" si="5"/>
+        <v>376</v>
+      </c>
+      <c r="NN5">
+        <f t="shared" si="5"/>
+        <v>377</v>
+      </c>
+      <c r="NO5">
+        <f t="shared" si="5"/>
+        <v>378</v>
+      </c>
+      <c r="NP5">
+        <f t="shared" si="5"/>
+        <v>379</v>
+      </c>
+      <c r="NQ5">
+        <f t="shared" si="5"/>
+        <v>380</v>
+      </c>
+      <c r="NR5">
+        <f t="shared" si="5"/>
+        <v>381</v>
+      </c>
+      <c r="NS5">
+        <f t="shared" si="5"/>
+        <v>382</v>
+      </c>
+      <c r="NT5">
+        <f t="shared" si="5"/>
+        <v>383</v>
+      </c>
+      <c r="NU5">
+        <f t="shared" si="5"/>
+        <v>384</v>
+      </c>
+      <c r="NV5">
+        <f t="shared" si="5"/>
+        <v>385</v>
+      </c>
+      <c r="NW5">
+        <f t="shared" si="5"/>
+        <v>386</v>
+      </c>
+      <c r="NX5">
+        <f t="shared" ref="NX5:OA5" si="6">NW5+1</f>
+        <v>387</v>
+      </c>
+      <c r="NY5">
+        <f t="shared" si="6"/>
+        <v>388</v>
+      </c>
+      <c r="NZ5">
+        <f t="shared" si="6"/>
+        <v>389</v>
+      </c>
+      <c r="OA5">
+        <f t="shared" si="6"/>
+        <v>390</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Canbus0_real. Update sevcon in components.xlsx
</commit_message>
<xml_diff>
--- a/src/main/java/ApplicationLayer/AppComponents/ExcelToAppComponent/Eolian_auriga/components.xlsx
+++ b/src/main/java/ApplicationLayer/AppComponents/ExcelToAppComponent/Eolian_auriga/components.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Github\Eolian\Eolian-Auriga-backend\src\main\java\ApplicationLayer\AppComponents\ExcelToAppComponent\Eolian_auriga\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3F06953-C591-4AE3-8BF1-2E7AB9DF1CF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14767FD7-5520-4615-B62A-B68BDFBB25B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mppt1" sheetId="7" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="luces" sheetId="11" r:id="rId5"/>
     <sheet name="gps" sheetId="15" r:id="rId6"/>
     <sheet name="acelerometro" sheetId="14" r:id="rId7"/>
+    <sheet name="sevcon" sheetId="16" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="457">
   <si>
     <t>Luz_alta</t>
   </si>
@@ -1315,6 +1316,102 @@
   </si>
   <si>
     <t>Disharge_overcurrent</t>
+  </si>
+  <si>
+    <t>der_motor_I</t>
+  </si>
+  <si>
+    <t>der_motor_RPM</t>
+  </si>
+  <si>
+    <t>der_battery_V</t>
+  </si>
+  <si>
+    <t>der_battery_I</t>
+  </si>
+  <si>
+    <t>der_inverter_temp</t>
+  </si>
+  <si>
+    <t>der_throttle_V</t>
+  </si>
+  <si>
+    <t>izq_motor_I</t>
+  </si>
+  <si>
+    <t>izq_motor_RPM</t>
+  </si>
+  <si>
+    <t>izq_battery_V</t>
+  </si>
+  <si>
+    <t>izq_battery_I</t>
+  </si>
+  <si>
+    <t>izq_inverter_temp</t>
+  </si>
+  <si>
+    <t>izq_throttle_V</t>
+  </si>
+  <si>
+    <t>der_target_I_quadrature</t>
+  </si>
+  <si>
+    <t>der_I_quadrature</t>
+  </si>
+  <si>
+    <t>der_V_quadrature</t>
+  </si>
+  <si>
+    <t>der_V_direct</t>
+  </si>
+  <si>
+    <t>der_target_I_direct</t>
+  </si>
+  <si>
+    <t>der_I_direct</t>
+  </si>
+  <si>
+    <t>izq_target_I_quadrature</t>
+  </si>
+  <si>
+    <t>izq_I_quadrature</t>
+  </si>
+  <si>
+    <t>izq_V_quadrature</t>
+  </si>
+  <si>
+    <t>izq_V_direct</t>
+  </si>
+  <si>
+    <t>izq_target_I_direct</t>
+  </si>
+  <si>
+    <t>izq_I_direct</t>
+  </si>
+  <si>
+    <t>der_motor_torque_demand</t>
+  </si>
+  <si>
+    <t>der_torque_actual</t>
+  </si>
+  <si>
+    <t>der_target_torque_percentaje</t>
+  </si>
+  <si>
+    <t>der_footbrake_V</t>
+  </si>
+  <si>
+    <t>izq_motor_torque_demand</t>
+  </si>
+  <si>
+    <t>izq_torque_actual</t>
+  </si>
+  <si>
+    <t>izq_target_torque_percentaje</t>
+  </si>
+  <si>
+    <t>izq_footbrake_V</t>
   </si>
 </sst>
 </file>
@@ -1350,10 +1447,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1640,7 +1738,7 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1733,7 +1831,7 @@
       <selection sqref="A1:H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1822,11 +1920,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72B547D1-632A-4F3B-9A3A-887796921B5F}">
   <dimension ref="A1:OA6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="AB1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="BD1" sqref="BD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:391" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -7362,7 +7460,7 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -7392,7 +7490,7 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -7467,7 +7565,7 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -7533,7 +7631,7 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -7566,6 +7664,582 @@
       </c>
       <c r="C3">
         <v>364</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04F22EE8-D25A-41DD-ADCF-948242599901}">
+  <dimension ref="A1:AF8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R13" sqref="R13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>427</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>425</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>449</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>426</v>
+      </c>
+      <c r="G1" t="s">
+        <v>437</v>
+      </c>
+      <c r="H1" t="s">
+        <v>438</v>
+      </c>
+      <c r="I1" t="s">
+        <v>450</v>
+      </c>
+      <c r="J1" t="s">
+        <v>439</v>
+      </c>
+      <c r="K1" t="s">
+        <v>430</v>
+      </c>
+      <c r="L1" t="s">
+        <v>441</v>
+      </c>
+      <c r="M1" t="s">
+        <v>442</v>
+      </c>
+      <c r="N1" t="s">
+        <v>440</v>
+      </c>
+      <c r="O1" t="s">
+        <v>451</v>
+      </c>
+      <c r="P1" t="s">
+        <v>452</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>434</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>435</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>431</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="W1" t="s">
+        <v>443</v>
+      </c>
+      <c r="X1" t="s">
+        <v>444</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>454</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>445</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>436</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>447</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>448</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>446</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>455</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>50.01</v>
+      </c>
+      <c r="B2">
+        <v>-100.01</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>-100.01</v>
+      </c>
+      <c r="E2">
+        <v>-150.01</v>
+      </c>
+      <c r="F2">
+        <v>-999.01</v>
+      </c>
+      <c r="G2">
+        <v>-200.01</v>
+      </c>
+      <c r="H2">
+        <v>-200.01</v>
+      </c>
+      <c r="I2">
+        <v>-150.01</v>
+      </c>
+      <c r="J2">
+        <v>-200.01</v>
+      </c>
+      <c r="K2">
+        <v>-0.99</v>
+      </c>
+      <c r="L2">
+        <v>-200.01</v>
+      </c>
+      <c r="M2">
+        <v>-200.01</v>
+      </c>
+      <c r="N2">
+        <v>-200.01</v>
+      </c>
+      <c r="O2">
+        <v>-0.99</v>
+      </c>
+      <c r="P2">
+        <v>-0.99</v>
+      </c>
+      <c r="Q2">
+        <v>50.01</v>
+      </c>
+      <c r="R2">
+        <v>-100.01</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>-100.01</v>
+      </c>
+      <c r="U2">
+        <v>-150.01</v>
+      </c>
+      <c r="V2">
+        <v>-999.01</v>
+      </c>
+      <c r="W2">
+        <v>-200.01</v>
+      </c>
+      <c r="X2">
+        <v>-200.01</v>
+      </c>
+      <c r="Y2">
+        <v>-150.01</v>
+      </c>
+      <c r="Z2">
+        <v>-200.01</v>
+      </c>
+      <c r="AA2">
+        <v>-0.99</v>
+      </c>
+      <c r="AB2">
+        <v>-200.01</v>
+      </c>
+      <c r="AC2">
+        <v>-200.01</v>
+      </c>
+      <c r="AD2">
+        <v>-200.01</v>
+      </c>
+      <c r="AE2">
+        <v>-0.99</v>
+      </c>
+      <c r="AF2">
+        <v>-0.99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>120.01</v>
+      </c>
+      <c r="B3">
+        <v>100.01</v>
+      </c>
+      <c r="C3">
+        <v>255</v>
+      </c>
+      <c r="D3">
+        <v>100.01</v>
+      </c>
+      <c r="E3">
+        <v>150.01</v>
+      </c>
+      <c r="F3">
+        <v>999.01</v>
+      </c>
+      <c r="G3">
+        <v>200.01</v>
+      </c>
+      <c r="H3">
+        <v>200.01</v>
+      </c>
+      <c r="I3">
+        <v>150.01</v>
+      </c>
+      <c r="J3">
+        <v>200.01</v>
+      </c>
+      <c r="K3">
+        <v>10.01</v>
+      </c>
+      <c r="L3">
+        <v>200.01</v>
+      </c>
+      <c r="M3">
+        <v>200.01</v>
+      </c>
+      <c r="N3">
+        <v>200.01</v>
+      </c>
+      <c r="O3">
+        <v>100.01</v>
+      </c>
+      <c r="P3">
+        <v>10.01</v>
+      </c>
+      <c r="Q3">
+        <v>120.01</v>
+      </c>
+      <c r="R3">
+        <v>100.01</v>
+      </c>
+      <c r="S3">
+        <v>255</v>
+      </c>
+      <c r="T3">
+        <v>100.01</v>
+      </c>
+      <c r="U3">
+        <v>150.01</v>
+      </c>
+      <c r="V3">
+        <v>999.01</v>
+      </c>
+      <c r="W3">
+        <v>200.01</v>
+      </c>
+      <c r="X3">
+        <v>200.01</v>
+      </c>
+      <c r="Y3">
+        <v>150.01</v>
+      </c>
+      <c r="Z3">
+        <v>200.01</v>
+      </c>
+      <c r="AA3">
+        <v>10.01</v>
+      </c>
+      <c r="AB3">
+        <v>200.01</v>
+      </c>
+      <c r="AC3">
+        <v>200.01</v>
+      </c>
+      <c r="AD3">
+        <v>200.01</v>
+      </c>
+      <c r="AE3">
+        <v>100.01</v>
+      </c>
+      <c r="AF3">
+        <v>10.01</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <f>F4+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <f>A4+1</f>
+        <v>4</v>
+      </c>
+      <c r="C4" s="3">
+        <f>B4+1</f>
+        <v>5</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3">
+        <f>D4+1</f>
+        <v>1</v>
+      </c>
+      <c r="F4" s="3">
+        <f>E4+1</f>
+        <v>2</v>
+      </c>
+      <c r="G4" s="3">
+        <f>C4+1</f>
+        <v>6</v>
+      </c>
+      <c r="H4" s="3">
+        <f t="shared" ref="C4:AB4" si="0">G4+1</f>
+        <v>7</v>
+      </c>
+      <c r="I4" s="3">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="J4" s="3">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="K4" s="3">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="L4" s="3">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="M4" s="3">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="N4" s="3">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="O4" s="3">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="P4" s="3">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="Q4" s="3">
+        <f>V4+1</f>
+        <v>19</v>
+      </c>
+      <c r="R4" s="3">
+        <f>Q4+1</f>
+        <v>20</v>
+      </c>
+      <c r="S4" s="3">
+        <f>R4+1</f>
+        <v>21</v>
+      </c>
+      <c r="T4" s="3">
+        <f>P4+1</f>
+        <v>16</v>
+      </c>
+      <c r="U4" s="3">
+        <f>T4+1</f>
+        <v>17</v>
+      </c>
+      <c r="V4" s="3">
+        <f>U4+1</f>
+        <v>18</v>
+      </c>
+      <c r="W4" s="3">
+        <f>S4+1</f>
+        <v>22</v>
+      </c>
+      <c r="X4" s="3">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="Y4" s="3">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="Z4" s="3">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="AA4" s="3">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="AB4" s="3">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="AC4" s="3">
+        <f t="shared" ref="AC4" si="1">AB4+1</f>
+        <v>28</v>
+      </c>
+      <c r="AD4" s="3">
+        <f t="shared" ref="AD4" si="2">AC4+1</f>
+        <v>29</v>
+      </c>
+      <c r="AE4" s="3">
+        <f t="shared" ref="AE4" si="3">AD4+1</f>
+        <v>30</v>
+      </c>
+      <c r="AF4" s="3">
+        <f t="shared" ref="AF4" si="4">AE4+1</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>100</v>
+      </c>
+      <c r="D6" s="3">
+        <v>200</v>
+      </c>
+      <c r="G6">
+        <v>300</v>
+      </c>
+      <c r="K6">
+        <v>400</v>
+      </c>
+      <c r="O6">
+        <v>500</v>
+      </c>
+      <c r="Q6">
+        <v>102</v>
+      </c>
+      <c r="T6">
+        <v>202</v>
+      </c>
+      <c r="W6">
+        <v>302</v>
+      </c>
+      <c r="AA6">
+        <v>402</v>
+      </c>
+      <c r="AE6">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>4</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
+      <c r="H8">
+        <v>2</v>
+      </c>
+      <c r="I8">
+        <v>2</v>
+      </c>
+      <c r="J8">
+        <v>2</v>
+      </c>
+      <c r="K8">
+        <v>2</v>
+      </c>
+      <c r="L8">
+        <v>2</v>
+      </c>
+      <c r="M8">
+        <v>2</v>
+      </c>
+      <c r="N8">
+        <v>2</v>
+      </c>
+      <c r="O8">
+        <v>2</v>
+      </c>
+      <c r="P8">
+        <v>2</v>
+      </c>
+      <c r="Q8">
+        <v>2</v>
+      </c>
+      <c r="R8">
+        <v>2</v>
+      </c>
+      <c r="S8">
+        <v>1</v>
+      </c>
+      <c r="T8">
+        <v>2</v>
+      </c>
+      <c r="U8">
+        <v>2</v>
+      </c>
+      <c r="V8">
+        <v>4</v>
+      </c>
+      <c r="W8">
+        <v>2</v>
+      </c>
+      <c r="X8">
+        <v>2</v>
+      </c>
+      <c r="Y8">
+        <v>2</v>
+      </c>
+      <c r="Z8">
+        <v>2</v>
+      </c>
+      <c r="AA8">
+        <v>2</v>
+      </c>
+      <c r="AB8">
+        <v>2</v>
+      </c>
+      <c r="AC8">
+        <v>2</v>
+      </c>
+      <c r="AD8">
+        <v>2</v>
+      </c>
+      <c r="AE8">
+        <v>2</v>
+      </c>
+      <c r="AF8">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix bugs, update some files
</commit_message>
<xml_diff>
--- a/src/main/java/ApplicationLayer/AppComponents/ExcelToAppComponent/Eolian_auriga/components.xlsx
+++ b/src/main/java/ApplicationLayer/AppComponents/ExcelToAppComponent/Eolian_auriga/components.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Github\Eolian\Eolian-Auriga-backend\src\main\java\ApplicationLayer\AppComponents\ExcelToAppComponent\Eolian_auriga\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14767FD7-5520-4615-B62A-B68BDFBB25B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C510E838-E45F-47A8-BE23-30E98E936288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="16080" windowWidth="29040" windowHeight="16440" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mppt1" sheetId="7" r:id="rId1"/>
@@ -1732,10 +1732,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60ED005C-EE4F-4655-A412-314A8EE2E525}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1816,6 +1816,38 @@
       </c>
       <c r="H3" s="1">
         <v>255</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <f>+B4+1</f>
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:H4" si="0">+C4+1</f>
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -1920,8 +1952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72B547D1-632A-4F3B-9A3A-887796921B5F}">
   <dimension ref="A1:OA6"/>
   <sheetViews>
-    <sheetView topLeftCell="AB1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="BD1" sqref="BD1"/>
+    <sheetView topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AE1" sqref="AE1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7676,7 +7708,7 @@
   <dimension ref="A1:AF8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7700,34 +7732,34 @@
       <c r="F1" s="3" t="s">
         <v>426</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="3" t="s">
         <v>437</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="3" t="s">
         <v>438</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="3" t="s">
         <v>450</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="3" t="s">
         <v>439</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="3" t="s">
         <v>430</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="3" t="s">
         <v>441</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="3" t="s">
         <v>442</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="3" t="s">
         <v>440</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="3" t="s">
         <v>451</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="3" t="s">
         <v>452</v>
       </c>
       <c r="Q1" s="3" t="s">
@@ -7780,52 +7812,52 @@
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="3">
         <v>50.01</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="3">
         <v>-100.01</v>
       </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
+      <c r="C2" s="3">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3">
         <v>-100.01</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="3">
         <v>-150.01</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="3">
         <v>-999.01</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="3">
         <v>-200.01</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="3">
         <v>-200.01</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="3">
         <v>-150.01</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="3">
         <v>-200.01</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="3">
         <v>-0.99</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="3">
         <v>-200.01</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="3">
         <v>-200.01</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="3">
         <v>-200.01</v>
       </c>
-      <c r="O2">
+      <c r="O2" s="3">
         <v>-0.99</v>
       </c>
-      <c r="P2">
+      <c r="P2" s="3">
         <v>-0.99</v>
       </c>
       <c r="Q2">
@@ -7878,52 +7910,52 @@
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="3">
         <v>120.01</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="3">
         <v>100.01</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="3">
         <v>255</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="3">
         <v>100.01</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="3">
         <v>150.01</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="3">
         <v>999.01</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="3">
         <v>200.01</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="3">
         <v>200.01</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="3">
         <v>150.01</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="3">
         <v>200.01</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="3">
         <v>10.01</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="3">
         <v>200.01</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="3">
         <v>200.01</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="3">
         <v>200.01</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="3">
         <v>100.01</v>
       </c>
-      <c r="P3">
+      <c r="P3" s="3">
         <v>10.01</v>
       </c>
       <c r="Q3">
@@ -7977,34 +8009,34 @@
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
-        <f>F4+1</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B4" s="3">
         <f>A4+1</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C4" s="3">
         <f>B4+1</f>
+        <v>2</v>
+      </c>
+      <c r="D4" s="3">
+        <f t="shared" ref="D4:AF4" si="0">C4+1</f>
+        <v>3</v>
+      </c>
+      <c r="E4" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F4" s="3">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="D4" s="3">
-        <v>0</v>
-      </c>
-      <c r="E4" s="3">
-        <f>D4+1</f>
-        <v>1</v>
-      </c>
-      <c r="F4" s="3">
-        <f>E4+1</f>
-        <v>2</v>
-      </c>
       <c r="G4" s="3">
-        <f>C4+1</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="H4" s="3">
-        <f t="shared" ref="C4:AB4" si="0">G4+1</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="I4" s="3">
@@ -8040,31 +8072,31 @@
         <v>15</v>
       </c>
       <c r="Q4" s="3">
-        <f>V4+1</f>
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="R4" s="3">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="S4" s="3">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="T4" s="3">
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="R4" s="3">
-        <f>Q4+1</f>
+      <c r="U4" s="3">
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="S4" s="3">
-        <f>R4+1</f>
+      <c r="V4" s="3">
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="T4" s="3">
-        <f>P4+1</f>
-        <v>16</v>
-      </c>
-      <c r="U4" s="3">
-        <f>T4+1</f>
-        <v>17</v>
-      </c>
-      <c r="V4" s="3">
-        <f>U4+1</f>
-        <v>18</v>
-      </c>
       <c r="W4" s="3">
-        <f>S4+1</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="X4" s="3">
@@ -8088,19 +8120,19 @@
         <v>27</v>
       </c>
       <c r="AC4" s="3">
-        <f t="shared" ref="AC4" si="1">AB4+1</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="AD4" s="3">
-        <f t="shared" ref="AD4" si="2">AC4+1</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="AE4" s="3">
-        <f t="shared" ref="AE4" si="3">AD4+1</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="AF4" s="3">
-        <f t="shared" ref="AF4" si="4">AE4+1</f>
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
     </row>
@@ -8111,6 +8143,16 @@
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6">

</xml_diff>